<commit_message>
Aggiornamento del file Catalogs.xlsx
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/Catalogs.xlsx
+++ b/apps/static/assets/dbs/Catalogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FA6135-94E2-EA40-ABCB-6F340298C23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E25D06F-D41A-2843-997F-DD5D4833A695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5720" uniqueCount="1642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5957" uniqueCount="1644">
   <si>
     <t>TID</t>
   </si>
@@ -5097,12 +5097,18 @@
 UNWIND target1_data + target2_data AS component_data
 RETURN component_data.component_id AS component_id, component_data.parameters AS parameters</t>
   </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5254,8 +5260,15 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF548235"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5304,8 +5317,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -5413,11 +5432,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9BC2E6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF9BC2E6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5581,6 +5633,48 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12349,16 +12443,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:Z393" totalsRowShown="0" dataDxfId="46">
-  <autoFilter ref="A1:Z393" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Network"/>
-        <filter val="Network.Core"/>
-        <filter val="Network.WiFi"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:Z408" totalsRowShown="0" dataDxfId="46">
+  <autoFilter ref="A1:Z408" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A255:R269">
     <sortCondition ref="B1:B313"/>
   </sortState>
@@ -12767,11 +12853,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Z393"/>
+  <dimension ref="A1:Z408"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B396" sqref="B396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12875,7 +12961,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="48" hidden="1">
+    <row r="2" spans="1:26" ht="48">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A64" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -12936,7 +13022,7 @@
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
     </row>
-    <row r="3" spans="1:26" ht="32" hidden="1">
+    <row r="3" spans="1:26" ht="32">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -12997,7 +13083,7 @@
       <c r="Y3" s="20"/>
       <c r="Z3" s="20"/>
     </row>
-    <row r="4" spans="1:26" ht="80" hidden="1">
+    <row r="4" spans="1:26" ht="80">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -13058,7 +13144,7 @@
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
     </row>
-    <row r="5" spans="1:26" ht="32" hidden="1">
+    <row r="5" spans="1:26" ht="32">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -13119,7 +13205,7 @@
       <c r="Y5" s="20"/>
       <c r="Z5" s="20"/>
     </row>
-    <row r="6" spans="1:26" ht="48" hidden="1">
+    <row r="6" spans="1:26" ht="48">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -13180,7 +13266,7 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="20"/>
     </row>
-    <row r="7" spans="1:26" ht="48" hidden="1">
+    <row r="7" spans="1:26" ht="48">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -13241,7 +13327,7 @@
       <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
     </row>
-    <row r="8" spans="1:26" ht="48" hidden="1">
+    <row r="8" spans="1:26" ht="48">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -13302,7 +13388,7 @@
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
     </row>
-    <row r="9" spans="1:26" ht="16" hidden="1">
+    <row r="9" spans="1:26" ht="16">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -13363,7 +13449,7 @@
       <c r="Y9" s="20"/>
       <c r="Z9" s="20"/>
     </row>
-    <row r="10" spans="1:26" ht="32" hidden="1">
+    <row r="10" spans="1:26" ht="32">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -13424,7 +13510,7 @@
       <c r="Y10" s="20"/>
       <c r="Z10" s="20"/>
     </row>
-    <row r="11" spans="1:26" ht="32" hidden="1">
+    <row r="11" spans="1:26" ht="32">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -13485,7 +13571,7 @@
       <c r="Y11" s="20"/>
       <c r="Z11" s="20"/>
     </row>
-    <row r="12" spans="1:26" ht="48" hidden="1">
+    <row r="12" spans="1:26" ht="48">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -13546,7 +13632,7 @@
       <c r="Y12" s="20"/>
       <c r="Z12" s="20"/>
     </row>
-    <row r="13" spans="1:26" ht="64" hidden="1">
+    <row r="13" spans="1:26" ht="64">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -13607,7 +13693,7 @@
       <c r="Y13" s="20"/>
       <c r="Z13" s="20"/>
     </row>
-    <row r="14" spans="1:26" ht="48" hidden="1">
+    <row r="14" spans="1:26" ht="48">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -13668,7 +13754,7 @@
       <c r="Y14" s="20"/>
       <c r="Z14" s="20"/>
     </row>
-    <row r="15" spans="1:26" ht="80" hidden="1">
+    <row r="15" spans="1:26" ht="80">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -13729,7 +13815,7 @@
       <c r="Y15" s="20"/>
       <c r="Z15" s="20"/>
     </row>
-    <row r="16" spans="1:26" ht="32" hidden="1">
+    <row r="16" spans="1:26" ht="32">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -13790,7 +13876,7 @@
       <c r="Y16" s="20"/>
       <c r="Z16" s="20"/>
     </row>
-    <row r="17" spans="1:26" ht="32" hidden="1">
+    <row r="17" spans="1:26" ht="32">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -13851,7 +13937,7 @@
       <c r="Y17" s="20"/>
       <c r="Z17" s="20"/>
     </row>
-    <row r="18" spans="1:26" ht="48" hidden="1">
+    <row r="18" spans="1:26" ht="48">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -13912,7 +13998,7 @@
       <c r="Y18" s="20"/>
       <c r="Z18" s="20"/>
     </row>
-    <row r="19" spans="1:26" ht="32" hidden="1">
+    <row r="19" spans="1:26" ht="32">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -13973,7 +14059,7 @@
       <c r="Y19" s="20"/>
       <c r="Z19" s="20"/>
     </row>
-    <row r="20" spans="1:26" ht="48" hidden="1">
+    <row r="20" spans="1:26" ht="48">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -14034,7 +14120,7 @@
       <c r="Y20" s="20"/>
       <c r="Z20" s="20"/>
     </row>
-    <row r="21" spans="1:26" ht="48" hidden="1">
+    <row r="21" spans="1:26" ht="48">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -14095,7 +14181,7 @@
       <c r="Y21" s="20"/>
       <c r="Z21" s="20"/>
     </row>
-    <row r="22" spans="1:26" ht="48" hidden="1">
+    <row r="22" spans="1:26" ht="48">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -14156,7 +14242,7 @@
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
     </row>
-    <row r="23" spans="1:26" ht="48" hidden="1">
+    <row r="23" spans="1:26" ht="48">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -14217,7 +14303,7 @@
       <c r="Y23" s="20"/>
       <c r="Z23" s="20"/>
     </row>
-    <row r="24" spans="1:26" ht="48" hidden="1">
+    <row r="24" spans="1:26" ht="48">
       <c r="A24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T23</v>
@@ -14281,7 +14367,7 @@
       <c r="Y24" s="20"/>
       <c r="Z24" s="20"/>
     </row>
-    <row r="25" spans="1:26" ht="48" hidden="1">
+    <row r="25" spans="1:26" ht="48">
       <c r="A25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T24</v>
@@ -14339,7 +14425,7 @@
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
     </row>
-    <row r="26" spans="1:26" ht="48" hidden="1">
+    <row r="26" spans="1:26" ht="48">
       <c r="A26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T25</v>
@@ -14397,7 +14483,7 @@
       <c r="Y26" s="20"/>
       <c r="Z26" s="20"/>
     </row>
-    <row r="27" spans="1:26" ht="64" hidden="1">
+    <row r="27" spans="1:26" ht="64">
       <c r="A27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T26</v>
@@ -14455,7 +14541,7 @@
       <c r="Y27" s="20"/>
       <c r="Z27" s="20"/>
     </row>
-    <row r="28" spans="1:26" ht="32" hidden="1">
+    <row r="28" spans="1:26" ht="32">
       <c r="A28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T27</v>
@@ -14513,7 +14599,7 @@
       <c r="Y28" s="20"/>
       <c r="Z28" s="20"/>
     </row>
-    <row r="29" spans="1:26" ht="48" hidden="1">
+    <row r="29" spans="1:26" ht="48">
       <c r="A29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T28</v>
@@ -14571,7 +14657,7 @@
       <c r="Y29" s="20"/>
       <c r="Z29" s="20"/>
     </row>
-    <row r="30" spans="1:26" ht="48" hidden="1">
+    <row r="30" spans="1:26" ht="48">
       <c r="A30" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T29</v>
@@ -14629,7 +14715,7 @@
       <c r="Y30" s="20"/>
       <c r="Z30" s="20"/>
     </row>
-    <row r="31" spans="1:26" ht="32" hidden="1">
+    <row r="31" spans="1:26" ht="32">
       <c r="A31" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T30</v>
@@ -14687,7 +14773,7 @@
       <c r="Y31" s="20"/>
       <c r="Z31" s="20"/>
     </row>
-    <row r="32" spans="1:26" ht="48" hidden="1">
+    <row r="32" spans="1:26" ht="48">
       <c r="A32" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T31</v>
@@ -14745,7 +14831,7 @@
       <c r="Y32" s="20"/>
       <c r="Z32" s="20"/>
     </row>
-    <row r="33" spans="1:26" ht="32" hidden="1">
+    <row r="33" spans="1:26" ht="32">
       <c r="A33" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T32</v>
@@ -14803,7 +14889,7 @@
       <c r="Y33" s="20"/>
       <c r="Z33" s="20"/>
     </row>
-    <row r="34" spans="1:26" ht="32" hidden="1">
+    <row r="34" spans="1:26" ht="32">
       <c r="A34" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T33</v>
@@ -14861,7 +14947,7 @@
       <c r="Y34" s="20"/>
       <c r="Z34" s="20"/>
     </row>
-    <row r="35" spans="1:26" ht="48" hidden="1">
+    <row r="35" spans="1:26" ht="48">
       <c r="A35" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T34</v>
@@ -14919,7 +15005,7 @@
       <c r="Y35" s="20"/>
       <c r="Z35" s="20"/>
     </row>
-    <row r="36" spans="1:26" ht="32" hidden="1">
+    <row r="36" spans="1:26" ht="32">
       <c r="A36" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T35</v>
@@ -14977,7 +15063,7 @@
       <c r="Y36" s="20"/>
       <c r="Z36" s="20"/>
     </row>
-    <row r="37" spans="1:26" ht="16" hidden="1">
+    <row r="37" spans="1:26" ht="16">
       <c r="A37" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T36</v>
@@ -15035,7 +15121,7 @@
       <c r="Y37" s="20"/>
       <c r="Z37" s="20"/>
     </row>
-    <row r="38" spans="1:26" ht="16" hidden="1">
+    <row r="38" spans="1:26" ht="16">
       <c r="A38" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T37</v>
@@ -15093,7 +15179,7 @@
       <c r="Y38" s="20"/>
       <c r="Z38" s="20"/>
     </row>
-    <row r="39" spans="1:26" ht="32" hidden="1">
+    <row r="39" spans="1:26" ht="32">
       <c r="A39" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T38</v>
@@ -15151,7 +15237,7 @@
       <c r="Y39" s="20"/>
       <c r="Z39" s="20"/>
     </row>
-    <row r="40" spans="1:26" ht="32" hidden="1">
+    <row r="40" spans="1:26" ht="32">
       <c r="A40" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T39</v>
@@ -15209,7 +15295,7 @@
       <c r="Y40" s="20"/>
       <c r="Z40" s="20"/>
     </row>
-    <row r="41" spans="1:26" ht="48" hidden="1">
+    <row r="41" spans="1:26" ht="48">
       <c r="A41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T40</v>
@@ -15267,7 +15353,7 @@
       <c r="Y41" s="20"/>
       <c r="Z41" s="20"/>
     </row>
-    <row r="42" spans="1:26" ht="48" hidden="1">
+    <row r="42" spans="1:26" ht="48">
       <c r="A42" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T41</v>
@@ -15325,7 +15411,7 @@
       <c r="Y42" s="20"/>
       <c r="Z42" s="20"/>
     </row>
-    <row r="43" spans="1:26" ht="16" hidden="1">
+    <row r="43" spans="1:26" ht="16">
       <c r="A43" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T42</v>
@@ -15383,7 +15469,7 @@
       <c r="Y43" s="20"/>
       <c r="Z43" s="20"/>
     </row>
-    <row r="44" spans="1:26" ht="48" hidden="1">
+    <row r="44" spans="1:26" ht="48">
       <c r="A44" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T43</v>
@@ -15441,7 +15527,7 @@
       <c r="Y44" s="20"/>
       <c r="Z44" s="20"/>
     </row>
-    <row r="45" spans="1:26" ht="48" hidden="1">
+    <row r="45" spans="1:26" ht="48">
       <c r="A45" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T44</v>
@@ -15499,7 +15585,7 @@
       <c r="Y45" s="20"/>
       <c r="Z45" s="20"/>
     </row>
-    <row r="46" spans="1:26" ht="32" hidden="1">
+    <row r="46" spans="1:26" ht="32">
       <c r="A46" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T45</v>
@@ -15557,7 +15643,7 @@
       <c r="Y46" s="20"/>
       <c r="Z46" s="20"/>
     </row>
-    <row r="47" spans="1:26" ht="32" hidden="1">
+    <row r="47" spans="1:26" ht="32">
       <c r="A47" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T46</v>
@@ -15621,7 +15707,7 @@
       <c r="Y47" s="20"/>
       <c r="Z47" s="20"/>
     </row>
-    <row r="48" spans="1:26" ht="48" hidden="1">
+    <row r="48" spans="1:26" ht="48">
       <c r="A48" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T47</v>
@@ -15679,7 +15765,7 @@
       <c r="Y48" s="20"/>
       <c r="Z48" s="20"/>
     </row>
-    <row r="49" spans="1:26" ht="32" hidden="1">
+    <row r="49" spans="1:26" ht="32">
       <c r="A49" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T48</v>
@@ -15737,7 +15823,7 @@
       <c r="Y49" s="20"/>
       <c r="Z49" s="20"/>
     </row>
-    <row r="50" spans="1:26" ht="32" hidden="1">
+    <row r="50" spans="1:26" ht="32">
       <c r="A50" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T49</v>
@@ -15795,7 +15881,7 @@
       <c r="Y50" s="20"/>
       <c r="Z50" s="20"/>
     </row>
-    <row r="51" spans="1:26" ht="32" hidden="1">
+    <row r="51" spans="1:26" ht="32">
       <c r="A51" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T50</v>
@@ -15853,7 +15939,7 @@
       <c r="Y51" s="20"/>
       <c r="Z51" s="20"/>
     </row>
-    <row r="52" spans="1:26" ht="32" hidden="1">
+    <row r="52" spans="1:26" ht="32">
       <c r="A52" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T51</v>
@@ -15911,7 +15997,7 @@
       <c r="Y52" s="20"/>
       <c r="Z52" s="20"/>
     </row>
-    <row r="53" spans="1:26" ht="48" hidden="1">
+    <row r="53" spans="1:26" ht="48">
       <c r="A53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T52</v>
@@ -15969,7 +16055,7 @@
       <c r="Y53" s="20"/>
       <c r="Z53" s="20"/>
     </row>
-    <row r="54" spans="1:26" ht="32" hidden="1">
+    <row r="54" spans="1:26" ht="32">
       <c r="A54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T53</v>
@@ -16027,7 +16113,7 @@
       <c r="Y54" s="20"/>
       <c r="Z54" s="20"/>
     </row>
-    <row r="55" spans="1:26" ht="48" hidden="1">
+    <row r="55" spans="1:26" ht="48">
       <c r="A55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T54</v>
@@ -16085,7 +16171,7 @@
       <c r="Y55" s="20"/>
       <c r="Z55" s="20"/>
     </row>
-    <row r="56" spans="1:26" ht="32" hidden="1">
+    <row r="56" spans="1:26" ht="32">
       <c r="A56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T55</v>
@@ -16143,7 +16229,7 @@
       <c r="Y56" s="20"/>
       <c r="Z56" s="20"/>
     </row>
-    <row r="57" spans="1:26" ht="80" hidden="1">
+    <row r="57" spans="1:26" ht="80">
       <c r="A57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T56</v>
@@ -16201,7 +16287,7 @@
       <c r="Y57" s="20"/>
       <c r="Z57" s="20"/>
     </row>
-    <row r="58" spans="1:26" ht="32" hidden="1">
+    <row r="58" spans="1:26" ht="32">
       <c r="A58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T57</v>
@@ -16259,7 +16345,7 @@
       <c r="Y58" s="20"/>
       <c r="Z58" s="20"/>
     </row>
-    <row r="59" spans="1:26" ht="32" hidden="1">
+    <row r="59" spans="1:26" ht="32">
       <c r="A59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T58</v>
@@ -16317,7 +16403,7 @@
       <c r="Y59" s="20"/>
       <c r="Z59" s="20"/>
     </row>
-    <row r="60" spans="1:26" ht="64" hidden="1">
+    <row r="60" spans="1:26" ht="64">
       <c r="A60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T59</v>
@@ -16386,7 +16472,7 @@
       <c r="Y60" s="20"/>
       <c r="Z60" s="20"/>
     </row>
-    <row r="61" spans="1:26" ht="395" hidden="1">
+    <row r="61" spans="1:26" ht="395">
       <c r="A61" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T60</v>
@@ -16455,7 +16541,7 @@
       <c r="Y61" s="20"/>
       <c r="Z61" s="20"/>
     </row>
-    <row r="62" spans="1:26" ht="80" hidden="1">
+    <row r="62" spans="1:26" ht="80">
       <c r="A62" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T61</v>
@@ -16524,7 +16610,7 @@
       <c r="Y62" s="20"/>
       <c r="Z62" s="20"/>
     </row>
-    <row r="63" spans="1:26" ht="240" hidden="1">
+    <row r="63" spans="1:26" ht="240">
       <c r="A63" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T62</v>
@@ -16593,7 +16679,7 @@
       <c r="Y63" s="20"/>
       <c r="Z63" s="20"/>
     </row>
-    <row r="64" spans="1:26" ht="48" hidden="1">
+    <row r="64" spans="1:26" ht="48">
       <c r="A64" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T63</v>
@@ -16662,7 +16748,7 @@
       <c r="Y64" s="20"/>
       <c r="Z64" s="20"/>
     </row>
-    <row r="65" spans="1:26" ht="96" hidden="1">
+    <row r="65" spans="1:26" ht="96">
       <c r="A65" s="20" t="str">
         <f t="shared" ref="A65:A128" si="12">CONCATENATE("T",ROW(A65)-1)</f>
         <v>T64</v>
@@ -16733,7 +16819,7 @@
       <c r="Y65" s="20"/>
       <c r="Z65" s="20"/>
     </row>
-    <row r="66" spans="1:26" ht="256" hidden="1">
+    <row r="66" spans="1:26" ht="256">
       <c r="A66" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T65</v>
@@ -16802,7 +16888,7 @@
       <c r="Y66" s="20"/>
       <c r="Z66" s="20"/>
     </row>
-    <row r="67" spans="1:26" ht="16" hidden="1">
+    <row r="67" spans="1:26" ht="16">
       <c r="A67" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T66</v>
@@ -16867,7 +16953,7 @@
       <c r="Y67" s="20"/>
       <c r="Z67" s="20"/>
     </row>
-    <row r="68" spans="1:26" ht="112" hidden="1">
+    <row r="68" spans="1:26" ht="112">
       <c r="A68" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T67</v>
@@ -16938,7 +17024,7 @@
       <c r="Y68" s="20"/>
       <c r="Z68" s="20"/>
     </row>
-    <row r="69" spans="1:26" ht="144" hidden="1">
+    <row r="69" spans="1:26" ht="144">
       <c r="A69" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T68</v>
@@ -17007,7 +17093,7 @@
       <c r="Y69" s="20"/>
       <c r="Z69" s="20"/>
     </row>
-    <row r="70" spans="1:26" ht="96" hidden="1">
+    <row r="70" spans="1:26" ht="96">
       <c r="A70" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T69</v>
@@ -17076,7 +17162,7 @@
       <c r="Y70" s="20"/>
       <c r="Z70" s="20"/>
     </row>
-    <row r="71" spans="1:26" ht="48" hidden="1">
+    <row r="71" spans="1:26" ht="48">
       <c r="A71" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T70</v>
@@ -17141,7 +17227,7 @@
       <c r="Y71" s="20"/>
       <c r="Z71" s="20"/>
     </row>
-    <row r="72" spans="1:26" ht="48" hidden="1">
+    <row r="72" spans="1:26" ht="48">
       <c r="A72" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T71</v>
@@ -17210,7 +17296,7 @@
       <c r="Y72" s="20"/>
       <c r="Z72" s="20"/>
     </row>
-    <row r="73" spans="1:26" ht="48" hidden="1">
+    <row r="73" spans="1:26" ht="48">
       <c r="A73" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T72</v>
@@ -17279,7 +17365,7 @@
       <c r="Y73" s="20"/>
       <c r="Z73" s="20"/>
     </row>
-    <row r="74" spans="1:26" ht="32" hidden="1">
+    <row r="74" spans="1:26" ht="32">
       <c r="A74" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T73</v>
@@ -17348,7 +17434,7 @@
       <c r="Y74" s="20"/>
       <c r="Z74" s="20"/>
     </row>
-    <row r="75" spans="1:26" ht="80" hidden="1">
+    <row r="75" spans="1:26" ht="80">
       <c r="A75" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T74</v>
@@ -17417,7 +17503,7 @@
       <c r="Y75" s="20"/>
       <c r="Z75" s="20"/>
     </row>
-    <row r="76" spans="1:26" ht="160" hidden="1">
+    <row r="76" spans="1:26" ht="160">
       <c r="A76" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T75</v>
@@ -17486,7 +17572,7 @@
       <c r="Y76" s="20"/>
       <c r="Z76" s="20"/>
     </row>
-    <row r="77" spans="1:26" ht="128" hidden="1">
+    <row r="77" spans="1:26" ht="128">
       <c r="A77" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T76</v>
@@ -17553,7 +17639,7 @@
       <c r="Y77" s="20"/>
       <c r="Z77" s="20"/>
     </row>
-    <row r="78" spans="1:26" ht="80" hidden="1">
+    <row r="78" spans="1:26" ht="80">
       <c r="A78" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T77</v>
@@ -17622,7 +17708,7 @@
       <c r="Y78" s="20"/>
       <c r="Z78" s="20"/>
     </row>
-    <row r="79" spans="1:26" ht="96" hidden="1">
+    <row r="79" spans="1:26" ht="96">
       <c r="A79" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T78</v>
@@ -17691,7 +17777,7 @@
       <c r="Y79" s="20"/>
       <c r="Z79" s="20"/>
     </row>
-    <row r="80" spans="1:26" ht="96" hidden="1">
+    <row r="80" spans="1:26" ht="96">
       <c r="A80" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T79</v>
@@ -17760,7 +17846,7 @@
       <c r="Y80" s="20"/>
       <c r="Z80" s="20"/>
     </row>
-    <row r="81" spans="1:26" ht="240" hidden="1">
+    <row r="81" spans="1:26" ht="240">
       <c r="A81" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T80</v>
@@ -17829,7 +17915,7 @@
       <c r="Y81" s="20"/>
       <c r="Z81" s="20"/>
     </row>
-    <row r="82" spans="1:26" ht="32" hidden="1">
+    <row r="82" spans="1:26" ht="32">
       <c r="A82" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T81</v>
@@ -17888,7 +17974,7 @@
       <c r="Y82" s="20"/>
       <c r="Z82" s="20"/>
     </row>
-    <row r="83" spans="1:26" ht="16" hidden="1">
+    <row r="83" spans="1:26" ht="16">
       <c r="A83" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T82</v>
@@ -17947,7 +18033,7 @@
       <c r="Y83" s="20"/>
       <c r="Z83" s="20"/>
     </row>
-    <row r="84" spans="1:26" ht="16" hidden="1">
+    <row r="84" spans="1:26" ht="16">
       <c r="A84" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T83</v>
@@ -18006,7 +18092,7 @@
       <c r="Y84" s="20"/>
       <c r="Z84" s="20"/>
     </row>
-    <row r="85" spans="1:26" ht="96" hidden="1">
+    <row r="85" spans="1:26" ht="96">
       <c r="A85" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T84</v>
@@ -18065,7 +18151,7 @@
       <c r="Y85" s="20"/>
       <c r="Z85" s="20"/>
     </row>
-    <row r="86" spans="1:26" ht="64" hidden="1">
+    <row r="86" spans="1:26" ht="64">
       <c r="A86" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T85</v>
@@ -18124,7 +18210,7 @@
       <c r="Y86" s="20"/>
       <c r="Z86" s="20"/>
     </row>
-    <row r="87" spans="1:26" ht="32" hidden="1">
+    <row r="87" spans="1:26" ht="32">
       <c r="A87" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T86</v>
@@ -18183,7 +18269,7 @@
       <c r="Y87" s="20"/>
       <c r="Z87" s="20"/>
     </row>
-    <row r="88" spans="1:26" ht="16" hidden="1">
+    <row r="88" spans="1:26" ht="16">
       <c r="A88" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T87</v>
@@ -18242,7 +18328,7 @@
       <c r="Y88" s="20"/>
       <c r="Z88" s="20"/>
     </row>
-    <row r="89" spans="1:26" ht="32" hidden="1">
+    <row r="89" spans="1:26" ht="32">
       <c r="A89" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T88</v>
@@ -18301,7 +18387,7 @@
       <c r="Y89" s="20"/>
       <c r="Z89" s="20"/>
     </row>
-    <row r="90" spans="1:26" ht="48" hidden="1">
+    <row r="90" spans="1:26" ht="48">
       <c r="A90" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T89</v>
@@ -18360,7 +18446,7 @@
       <c r="Y90" s="20"/>
       <c r="Z90" s="20"/>
     </row>
-    <row r="91" spans="1:26" ht="96" hidden="1">
+    <row r="91" spans="1:26" ht="96">
       <c r="A91" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T90</v>
@@ -18419,7 +18505,7 @@
       <c r="Y91" s="20"/>
       <c r="Z91" s="20"/>
     </row>
-    <row r="92" spans="1:26" ht="64" hidden="1">
+    <row r="92" spans="1:26" ht="64">
       <c r="A92" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T91</v>
@@ -18478,7 +18564,7 @@
       <c r="Y92" s="20"/>
       <c r="Z92" s="20"/>
     </row>
-    <row r="93" spans="1:26" ht="48" hidden="1">
+    <row r="93" spans="1:26" ht="48">
       <c r="A93" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T92</v>
@@ -18537,7 +18623,7 @@
       <c r="Y93" s="20"/>
       <c r="Z93" s="20"/>
     </row>
-    <row r="94" spans="1:26" ht="32" hidden="1">
+    <row r="94" spans="1:26" ht="32">
       <c r="A94" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T93</v>
@@ -18596,7 +18682,7 @@
       <c r="Y94" s="20"/>
       <c r="Z94" s="20"/>
     </row>
-    <row r="95" spans="1:26" ht="32" hidden="1">
+    <row r="95" spans="1:26" ht="32">
       <c r="A95" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T94</v>
@@ -18655,7 +18741,7 @@
       <c r="Y95" s="20"/>
       <c r="Z95" s="20"/>
     </row>
-    <row r="96" spans="1:26" ht="32" hidden="1">
+    <row r="96" spans="1:26" ht="32">
       <c r="A96" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T95</v>
@@ -18714,7 +18800,7 @@
       <c r="Y96" s="20"/>
       <c r="Z96" s="20"/>
     </row>
-    <row r="97" spans="1:26" ht="64" hidden="1">
+    <row r="97" spans="1:26" ht="64">
       <c r="A97" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T96</v>
@@ -18773,7 +18859,7 @@
       <c r="Y97" s="20"/>
       <c r="Z97" s="20"/>
     </row>
-    <row r="98" spans="1:26" ht="48" hidden="1">
+    <row r="98" spans="1:26" ht="48">
       <c r="A98" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T97</v>
@@ -21579,7 +21665,7 @@
       <c r="Y136" s="61"/>
       <c r="Z136" s="61"/>
     </row>
-    <row r="137" spans="1:26" ht="96" hidden="1">
+    <row r="137" spans="1:26" ht="96">
       <c r="A137" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T136</v>
@@ -21638,7 +21724,7 @@
       <c r="Y137" s="61"/>
       <c r="Z137" s="61"/>
     </row>
-    <row r="138" spans="1:26" ht="80" hidden="1">
+    <row r="138" spans="1:26" ht="80">
       <c r="A138" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T137</v>
@@ -21697,7 +21783,7 @@
       <c r="Y138" s="61"/>
       <c r="Z138" s="61"/>
     </row>
-    <row r="139" spans="1:26" ht="96" hidden="1">
+    <row r="139" spans="1:26" ht="96">
       <c r="A139" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T138</v>
@@ -21756,7 +21842,7 @@
       <c r="Y139" s="61"/>
       <c r="Z139" s="61"/>
     </row>
-    <row r="140" spans="1:26" ht="48" hidden="1">
+    <row r="140" spans="1:26" ht="48">
       <c r="A140" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T139</v>
@@ -21815,7 +21901,7 @@
       <c r="Y140" s="61"/>
       <c r="Z140" s="61"/>
     </row>
-    <row r="141" spans="1:26" ht="80" hidden="1">
+    <row r="141" spans="1:26" ht="80">
       <c r="A141" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T140</v>
@@ -21874,7 +21960,7 @@
       <c r="Y141" s="61"/>
       <c r="Z141" s="61"/>
     </row>
-    <row r="142" spans="1:26" ht="48" hidden="1">
+    <row r="142" spans="1:26" ht="48">
       <c r="A142" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T141</v>
@@ -21933,7 +22019,7 @@
       <c r="Y142" s="61"/>
       <c r="Z142" s="61"/>
     </row>
-    <row r="143" spans="1:26" ht="32" hidden="1">
+    <row r="143" spans="1:26" ht="32">
       <c r="A143" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T142</v>
@@ -21992,7 +22078,7 @@
       <c r="Y143" s="61"/>
       <c r="Z143" s="61"/>
     </row>
-    <row r="144" spans="1:26" ht="32" hidden="1">
+    <row r="144" spans="1:26" ht="32">
       <c r="A144" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T143</v>
@@ -22051,7 +22137,7 @@
       <c r="Y144" s="61"/>
       <c r="Z144" s="61"/>
     </row>
-    <row r="145" spans="1:26" ht="80" hidden="1">
+    <row r="145" spans="1:26" ht="80">
       <c r="A145" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T144</v>
@@ -22110,7 +22196,7 @@
       <c r="Y145" s="61"/>
       <c r="Z145" s="61"/>
     </row>
-    <row r="146" spans="1:26" ht="64" hidden="1">
+    <row r="146" spans="1:26" ht="64">
       <c r="A146" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T145</v>
@@ -22169,7 +22255,7 @@
       <c r="Y146" s="61"/>
       <c r="Z146" s="61"/>
     </row>
-    <row r="147" spans="1:26" ht="64" hidden="1">
+    <row r="147" spans="1:26" ht="64">
       <c r="A147" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T146</v>
@@ -22228,7 +22314,7 @@
       <c r="Y147" s="61"/>
       <c r="Z147" s="61"/>
     </row>
-    <row r="148" spans="1:26" ht="32" hidden="1">
+    <row r="148" spans="1:26" ht="32">
       <c r="A148" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T147</v>
@@ -22287,7 +22373,7 @@
       <c r="Y148" s="61"/>
       <c r="Z148" s="61"/>
     </row>
-    <row r="149" spans="1:26" ht="64" hidden="1">
+    <row r="149" spans="1:26" ht="64">
       <c r="A149" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T148</v>
@@ -22346,7 +22432,7 @@
       <c r="Y149" s="61"/>
       <c r="Z149" s="61"/>
     </row>
-    <row r="150" spans="1:26" ht="112" hidden="1">
+    <row r="150" spans="1:26" ht="112">
       <c r="A150" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T149</v>
@@ -22405,7 +22491,7 @@
       <c r="Y150" s="61"/>
       <c r="Z150" s="61"/>
     </row>
-    <row r="151" spans="1:26" ht="64" hidden="1">
+    <row r="151" spans="1:26" ht="64">
       <c r="A151" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T150</v>
@@ -22464,7 +22550,7 @@
       <c r="Y151" s="61"/>
       <c r="Z151" s="61"/>
     </row>
-    <row r="152" spans="1:26" ht="96" hidden="1">
+    <row r="152" spans="1:26" ht="96">
       <c r="A152" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T151</v>
@@ -22523,7 +22609,7 @@
       <c r="Y152" s="61"/>
       <c r="Z152" s="61"/>
     </row>
-    <row r="153" spans="1:26" ht="160" hidden="1">
+    <row r="153" spans="1:26" ht="160">
       <c r="A153" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T152</v>
@@ -22582,7 +22668,7 @@
       <c r="Y153" s="61"/>
       <c r="Z153" s="61"/>
     </row>
-    <row r="154" spans="1:26" ht="96" hidden="1">
+    <row r="154" spans="1:26" ht="96">
       <c r="A154" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T153</v>
@@ -22641,7 +22727,7 @@
       <c r="Y154" s="61"/>
       <c r="Z154" s="61"/>
     </row>
-    <row r="155" spans="1:26" ht="80" hidden="1">
+    <row r="155" spans="1:26" ht="80">
       <c r="A155" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T154</v>
@@ -22700,7 +22786,7 @@
       <c r="Y155" s="61"/>
       <c r="Z155" s="61"/>
     </row>
-    <row r="156" spans="1:26" ht="96" hidden="1">
+    <row r="156" spans="1:26" ht="96">
       <c r="A156" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T155</v>
@@ -22759,7 +22845,7 @@
       <c r="Y156" s="61"/>
       <c r="Z156" s="61"/>
     </row>
-    <row r="157" spans="1:26" ht="48" hidden="1">
+    <row r="157" spans="1:26" ht="48">
       <c r="A157" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T156</v>
@@ -22818,7 +22904,7 @@
       <c r="Y157" s="61"/>
       <c r="Z157" s="61"/>
     </row>
-    <row r="158" spans="1:26" ht="32" hidden="1">
+    <row r="158" spans="1:26" ht="32">
       <c r="A158" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T157</v>
@@ -22877,7 +22963,7 @@
       <c r="Y158" s="61"/>
       <c r="Z158" s="61"/>
     </row>
-    <row r="159" spans="1:26" ht="80" hidden="1">
+    <row r="159" spans="1:26" ht="80">
       <c r="A159" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T158</v>
@@ -22936,7 +23022,7 @@
       <c r="Y159" s="61"/>
       <c r="Z159" s="61"/>
     </row>
-    <row r="160" spans="1:26" ht="80" hidden="1">
+    <row r="160" spans="1:26" ht="80">
       <c r="A160" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T159</v>
@@ -22995,7 +23081,7 @@
       <c r="Y160" s="61"/>
       <c r="Z160" s="61"/>
     </row>
-    <row r="161" spans="1:26" ht="64" hidden="1">
+    <row r="161" spans="1:26" ht="64">
       <c r="A161" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T160</v>
@@ -23054,7 +23140,7 @@
       <c r="Y161" s="61"/>
       <c r="Z161" s="61"/>
     </row>
-    <row r="162" spans="1:26" ht="64" hidden="1">
+    <row r="162" spans="1:26" ht="64">
       <c r="A162" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T161</v>
@@ -23113,7 +23199,7 @@
       <c r="Y162" s="61"/>
       <c r="Z162" s="61"/>
     </row>
-    <row r="163" spans="1:26" ht="48" hidden="1">
+    <row r="163" spans="1:26" ht="48">
       <c r="A163" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T162</v>
@@ -23172,7 +23258,7 @@
       <c r="Y163" s="61"/>
       <c r="Z163" s="61"/>
     </row>
-    <row r="164" spans="1:26" ht="32" hidden="1">
+    <row r="164" spans="1:26" ht="32">
       <c r="A164" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T163</v>
@@ -23231,7 +23317,7 @@
       <c r="Y164" s="61"/>
       <c r="Z164" s="61"/>
     </row>
-    <row r="165" spans="1:26" ht="32" hidden="1">
+    <row r="165" spans="1:26" ht="32">
       <c r="A165" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T164</v>
@@ -23290,7 +23376,7 @@
       <c r="Y165" s="61"/>
       <c r="Z165" s="61"/>
     </row>
-    <row r="166" spans="1:26" ht="32" hidden="1">
+    <row r="166" spans="1:26" ht="32">
       <c r="A166" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T165</v>
@@ -23349,7 +23435,7 @@
       <c r="Y166" s="61"/>
       <c r="Z166" s="61"/>
     </row>
-    <row r="167" spans="1:26" ht="32" hidden="1">
+    <row r="167" spans="1:26" ht="32">
       <c r="A167" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T166</v>
@@ -23408,7 +23494,7 @@
       <c r="Y167" s="61"/>
       <c r="Z167" s="61"/>
     </row>
-    <row r="168" spans="1:26" ht="64" hidden="1">
+    <row r="168" spans="1:26" ht="64">
       <c r="A168" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T167</v>
@@ -23467,7 +23553,7 @@
       <c r="Y168" s="61"/>
       <c r="Z168" s="61"/>
     </row>
-    <row r="169" spans="1:26" ht="48" hidden="1">
+    <row r="169" spans="1:26" ht="48">
       <c r="A169" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T168</v>
@@ -23526,7 +23612,7 @@
       <c r="Y169" s="61"/>
       <c r="Z169" s="61"/>
     </row>
-    <row r="170" spans="1:26" ht="32" hidden="1">
+    <row r="170" spans="1:26" ht="32">
       <c r="A170" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T169</v>
@@ -23585,7 +23671,7 @@
       <c r="Y170" s="61"/>
       <c r="Z170" s="61"/>
     </row>
-    <row r="171" spans="1:26" ht="32" hidden="1">
+    <row r="171" spans="1:26" ht="32">
       <c r="A171" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T170</v>
@@ -23644,7 +23730,7 @@
       <c r="Y171" s="61"/>
       <c r="Z171" s="61"/>
     </row>
-    <row r="172" spans="1:26" ht="16" hidden="1">
+    <row r="172" spans="1:26" ht="16">
       <c r="A172" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T171</v>
@@ -23703,7 +23789,7 @@
       <c r="Y172" s="61"/>
       <c r="Z172" s="61"/>
     </row>
-    <row r="173" spans="1:26" ht="16" hidden="1">
+    <row r="173" spans="1:26" ht="16">
       <c r="A173" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T172</v>
@@ -23762,7 +23848,7 @@
       <c r="Y173" s="61"/>
       <c r="Z173" s="61"/>
     </row>
-    <row r="174" spans="1:26" ht="64" hidden="1">
+    <row r="174" spans="1:26" ht="64">
       <c r="A174" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T173</v>
@@ -23821,7 +23907,7 @@
       <c r="Y174" s="61"/>
       <c r="Z174" s="61"/>
     </row>
-    <row r="175" spans="1:26" ht="64" hidden="1">
+    <row r="175" spans="1:26" ht="64">
       <c r="A175" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T174</v>
@@ -23880,7 +23966,7 @@
       <c r="Y175" s="61"/>
       <c r="Z175" s="61"/>
     </row>
-    <row r="176" spans="1:26" ht="80" hidden="1">
+    <row r="176" spans="1:26" ht="80">
       <c r="A176" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T175</v>
@@ -23939,7 +24025,7 @@
       <c r="Y176" s="61"/>
       <c r="Z176" s="61"/>
     </row>
-    <row r="177" spans="1:26" ht="48" hidden="1">
+    <row r="177" spans="1:26" ht="48">
       <c r="A177" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T176</v>
@@ -23998,7 +24084,7 @@
       <c r="Y177" s="61"/>
       <c r="Z177" s="61"/>
     </row>
-    <row r="178" spans="1:26" ht="32" hidden="1">
+    <row r="178" spans="1:26" ht="32">
       <c r="A178" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T177</v>
@@ -24057,7 +24143,7 @@
       <c r="Y178" s="61"/>
       <c r="Z178" s="61"/>
     </row>
-    <row r="179" spans="1:26" ht="32" hidden="1">
+    <row r="179" spans="1:26" ht="32">
       <c r="A179" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T178</v>
@@ -24116,7 +24202,7 @@
       <c r="Y179" s="61"/>
       <c r="Z179" s="61"/>
     </row>
-    <row r="180" spans="1:26" ht="80" hidden="1">
+    <row r="180" spans="1:26" ht="80">
       <c r="A180" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T179</v>
@@ -24175,7 +24261,7 @@
       <c r="Y180" s="61"/>
       <c r="Z180" s="61"/>
     </row>
-    <row r="181" spans="1:26" ht="64" hidden="1">
+    <row r="181" spans="1:26" ht="64">
       <c r="A181" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T180</v>
@@ -24234,7 +24320,7 @@
       <c r="Y181" s="61"/>
       <c r="Z181" s="61"/>
     </row>
-    <row r="182" spans="1:26" ht="64" hidden="1">
+    <row r="182" spans="1:26" ht="64">
       <c r="A182" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T181</v>
@@ -24293,7 +24379,7 @@
       <c r="Y182" s="61"/>
       <c r="Z182" s="61"/>
     </row>
-    <row r="183" spans="1:26" ht="144" hidden="1">
+    <row r="183" spans="1:26" ht="144">
       <c r="A183" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T182</v>
@@ -24352,7 +24438,7 @@
       <c r="Y183" s="61"/>
       <c r="Z183" s="61"/>
     </row>
-    <row r="184" spans="1:26" ht="96" hidden="1">
+    <row r="184" spans="1:26" ht="96">
       <c r="A184" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T183</v>
@@ -24411,7 +24497,7 @@
       <c r="Y184" s="61"/>
       <c r="Z184" s="61"/>
     </row>
-    <row r="185" spans="1:26" ht="48" hidden="1">
+    <row r="185" spans="1:26" ht="48">
       <c r="A185" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T184</v>
@@ -24470,7 +24556,7 @@
       <c r="Y185" s="61"/>
       <c r="Z185" s="61"/>
     </row>
-    <row r="186" spans="1:26" ht="16" hidden="1">
+    <row r="186" spans="1:26" ht="16">
       <c r="A186" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T185</v>
@@ -24529,7 +24615,7 @@
       <c r="Y186" s="61"/>
       <c r="Z186" s="61"/>
     </row>
-    <row r="187" spans="1:26" ht="144" hidden="1">
+    <row r="187" spans="1:26" ht="144">
       <c r="A187" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T186</v>
@@ -24588,7 +24674,7 @@
       <c r="Y187" s="61"/>
       <c r="Z187" s="61"/>
     </row>
-    <row r="188" spans="1:26" ht="128" hidden="1">
+    <row r="188" spans="1:26" ht="128">
       <c r="A188" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T187</v>
@@ -24647,7 +24733,7 @@
       <c r="Y188" s="61"/>
       <c r="Z188" s="61"/>
     </row>
-    <row r="189" spans="1:26" ht="128" hidden="1">
+    <row r="189" spans="1:26" ht="128">
       <c r="A189" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T188</v>
@@ -24706,7 +24792,7 @@
       <c r="Y189" s="61"/>
       <c r="Z189" s="61"/>
     </row>
-    <row r="190" spans="1:26" ht="96" hidden="1">
+    <row r="190" spans="1:26" ht="96">
       <c r="A190" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T189</v>
@@ -24765,7 +24851,7 @@
       <c r="Y190" s="61"/>
       <c r="Z190" s="61"/>
     </row>
-    <row r="191" spans="1:26" ht="80" hidden="1">
+    <row r="191" spans="1:26" ht="80">
       <c r="A191" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T190</v>
@@ -24824,7 +24910,7 @@
       <c r="Y191" s="61"/>
       <c r="Z191" s="61"/>
     </row>
-    <row r="192" spans="1:26" ht="80" hidden="1">
+    <row r="192" spans="1:26" ht="80">
       <c r="A192" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T191</v>
@@ -24883,7 +24969,7 @@
       <c r="Y192" s="61"/>
       <c r="Z192" s="61"/>
     </row>
-    <row r="193" spans="1:26" ht="48" hidden="1">
+    <row r="193" spans="1:26" ht="48">
       <c r="A193" s="20" t="str">
         <f t="shared" ref="A193:A254" si="28">CONCATENATE("T",ROW(A193)-1)</f>
         <v>T192</v>
@@ -24942,7 +25028,7 @@
       <c r="Y193" s="61"/>
       <c r="Z193" s="61"/>
     </row>
-    <row r="194" spans="1:26" ht="32" hidden="1">
+    <row r="194" spans="1:26" ht="32">
       <c r="A194" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T193</v>
@@ -25001,7 +25087,7 @@
       <c r="Y194" s="61"/>
       <c r="Z194" s="61"/>
     </row>
-    <row r="195" spans="1:26" ht="80" hidden="1">
+    <row r="195" spans="1:26" ht="80">
       <c r="A195" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T194</v>
@@ -25060,7 +25146,7 @@
       <c r="Y195" s="61"/>
       <c r="Z195" s="61"/>
     </row>
-    <row r="196" spans="1:26" ht="96" hidden="1">
+    <row r="196" spans="1:26" ht="96">
       <c r="A196" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T195</v>
@@ -25119,7 +25205,7 @@
       <c r="Y196" s="61"/>
       <c r="Z196" s="61"/>
     </row>
-    <row r="197" spans="1:26" ht="48" hidden="1">
+    <row r="197" spans="1:26" ht="48">
       <c r="A197" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T196</v>
@@ -25178,7 +25264,7 @@
       <c r="Y197" s="61"/>
       <c r="Z197" s="61"/>
     </row>
-    <row r="198" spans="1:26" ht="80" hidden="1">
+    <row r="198" spans="1:26" ht="80">
       <c r="A198" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T197</v>
@@ -25237,7 +25323,7 @@
       <c r="Y198" s="61"/>
       <c r="Z198" s="61"/>
     </row>
-    <row r="199" spans="1:26" ht="48" hidden="1">
+    <row r="199" spans="1:26" ht="48">
       <c r="A199" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T198</v>
@@ -25296,7 +25382,7 @@
       <c r="Y199" s="61"/>
       <c r="Z199" s="61"/>
     </row>
-    <row r="200" spans="1:26" ht="32" hidden="1">
+    <row r="200" spans="1:26" ht="32">
       <c r="A200" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T199</v>
@@ -25355,7 +25441,7 @@
       <c r="Y200" s="61"/>
       <c r="Z200" s="61"/>
     </row>
-    <row r="201" spans="1:26" ht="32" hidden="1">
+    <row r="201" spans="1:26" ht="32">
       <c r="A201" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T200</v>
@@ -25414,7 +25500,7 @@
       <c r="Y201" s="61"/>
       <c r="Z201" s="61"/>
     </row>
-    <row r="202" spans="1:26" ht="80" hidden="1">
+    <row r="202" spans="1:26" ht="80">
       <c r="A202" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T201</v>
@@ -25473,7 +25559,7 @@
       <c r="Y202" s="61"/>
       <c r="Z202" s="61"/>
     </row>
-    <row r="203" spans="1:26" ht="64" hidden="1">
+    <row r="203" spans="1:26" ht="64">
       <c r="A203" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T202</v>
@@ -25532,7 +25618,7 @@
       <c r="Y203" s="61"/>
       <c r="Z203" s="61"/>
     </row>
-    <row r="204" spans="1:26" ht="64" hidden="1">
+    <row r="204" spans="1:26" ht="64">
       <c r="A204" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T203</v>
@@ -25591,7 +25677,7 @@
       <c r="Y204" s="61"/>
       <c r="Z204" s="61"/>
     </row>
-    <row r="205" spans="1:26" ht="32" hidden="1">
+    <row r="205" spans="1:26" ht="32">
       <c r="A205" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T204</v>
@@ -25650,7 +25736,7 @@
       <c r="Y205" s="61"/>
       <c r="Z205" s="61"/>
     </row>
-    <row r="206" spans="1:26" ht="80" hidden="1">
+    <row r="206" spans="1:26" ht="80">
       <c r="A206" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T205</v>
@@ -25709,7 +25795,7 @@
       <c r="Y206" s="61"/>
       <c r="Z206" s="61"/>
     </row>
-    <row r="207" spans="1:26" ht="96" hidden="1">
+    <row r="207" spans="1:26" ht="96">
       <c r="A207" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T206</v>
@@ -25768,7 +25854,7 @@
       <c r="Y207" s="61"/>
       <c r="Z207" s="61"/>
     </row>
-    <row r="208" spans="1:26" ht="80" hidden="1">
+    <row r="208" spans="1:26" ht="80">
       <c r="A208" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T207</v>
@@ -25827,7 +25913,7 @@
       <c r="Y208" s="61"/>
       <c r="Z208" s="61"/>
     </row>
-    <row r="209" spans="1:26" ht="80" hidden="1">
+    <row r="209" spans="1:26" ht="80">
       <c r="A209" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T208</v>
@@ -25886,7 +25972,7 @@
       <c r="Y209" s="61"/>
       <c r="Z209" s="61"/>
     </row>
-    <row r="210" spans="1:26" ht="48" hidden="1">
+    <row r="210" spans="1:26" ht="48">
       <c r="A210" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T209</v>
@@ -25945,7 +26031,7 @@
       <c r="Y210" s="61"/>
       <c r="Z210" s="61"/>
     </row>
-    <row r="211" spans="1:26" ht="32" hidden="1">
+    <row r="211" spans="1:26" ht="32">
       <c r="A211" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T210</v>
@@ -26004,7 +26090,7 @@
       <c r="Y211" s="61"/>
       <c r="Z211" s="61"/>
     </row>
-    <row r="212" spans="1:26" ht="144" hidden="1">
+    <row r="212" spans="1:26" ht="144">
       <c r="A212" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T211</v>
@@ -26063,7 +26149,7 @@
       <c r="Y212" s="61"/>
       <c r="Z212" s="61"/>
     </row>
-    <row r="213" spans="1:26" ht="80" hidden="1">
+    <row r="213" spans="1:26" ht="80">
       <c r="A213" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T212</v>
@@ -26122,7 +26208,7 @@
       <c r="Y213" s="61"/>
       <c r="Z213" s="61"/>
     </row>
-    <row r="214" spans="1:26" ht="96" hidden="1">
+    <row r="214" spans="1:26" ht="96">
       <c r="A214" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T213</v>
@@ -26181,7 +26267,7 @@
       <c r="Y214" s="61"/>
       <c r="Z214" s="61"/>
     </row>
-    <row r="215" spans="1:26" ht="96" hidden="1">
+    <row r="215" spans="1:26" ht="96">
       <c r="A215" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T214</v>
@@ -26240,7 +26326,7 @@
       <c r="Y215" s="61"/>
       <c r="Z215" s="61"/>
     </row>
-    <row r="216" spans="1:26" ht="80" hidden="1">
+    <row r="216" spans="1:26" ht="80">
       <c r="A216" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T215</v>
@@ -26299,7 +26385,7 @@
       <c r="Y216" s="61"/>
       <c r="Z216" s="61"/>
     </row>
-    <row r="217" spans="1:26" ht="80" hidden="1">
+    <row r="217" spans="1:26" ht="80">
       <c r="A217" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T216</v>
@@ -26358,7 +26444,7 @@
       <c r="Y217" s="61"/>
       <c r="Z217" s="61"/>
     </row>
-    <row r="218" spans="1:26" ht="48" hidden="1">
+    <row r="218" spans="1:26" ht="48">
       <c r="A218" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T217</v>
@@ -26417,7 +26503,7 @@
       <c r="Y218" s="61"/>
       <c r="Z218" s="61"/>
     </row>
-    <row r="219" spans="1:26" ht="32" hidden="1">
+    <row r="219" spans="1:26" ht="32">
       <c r="A219" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T218</v>
@@ -26476,7 +26562,7 @@
       <c r="Y219" s="61"/>
       <c r="Z219" s="61"/>
     </row>
-    <row r="220" spans="1:26" ht="64" hidden="1">
+    <row r="220" spans="1:26" ht="64">
       <c r="A220" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T219</v>
@@ -26535,7 +26621,7 @@
       <c r="Y220" s="61"/>
       <c r="Z220" s="61"/>
     </row>
-    <row r="221" spans="1:26" ht="16" hidden="1">
+    <row r="221" spans="1:26" ht="16">
       <c r="A221" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T220</v>
@@ -26594,7 +26680,7 @@
       <c r="Y221" s="61"/>
       <c r="Z221" s="61"/>
     </row>
-    <row r="222" spans="1:26" ht="64" hidden="1">
+    <row r="222" spans="1:26" ht="64">
       <c r="A222" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T221</v>
@@ -26653,7 +26739,7 @@
       <c r="Y222" s="61"/>
       <c r="Z222" s="61"/>
     </row>
-    <row r="223" spans="1:26" ht="96" hidden="1">
+    <row r="223" spans="1:26" ht="96">
       <c r="A223" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T222</v>
@@ -26712,7 +26798,7 @@
       <c r="Y223" s="61"/>
       <c r="Z223" s="61"/>
     </row>
-    <row r="224" spans="1:26" ht="80" hidden="1">
+    <row r="224" spans="1:26" ht="80">
       <c r="A224" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T223</v>
@@ -26771,7 +26857,7 @@
       <c r="Y224" s="61"/>
       <c r="Z224" s="61"/>
     </row>
-    <row r="225" spans="1:26" ht="80" hidden="1">
+    <row r="225" spans="1:26" ht="80">
       <c r="A225" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T224</v>
@@ -26830,7 +26916,7 @@
       <c r="Y225" s="61"/>
       <c r="Z225" s="61"/>
     </row>
-    <row r="226" spans="1:26" ht="64" hidden="1">
+    <row r="226" spans="1:26" ht="64">
       <c r="A226" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T225</v>
@@ -26889,7 +26975,7 @@
       <c r="Y226" s="61"/>
       <c r="Z226" s="61"/>
     </row>
-    <row r="227" spans="1:26" ht="80" hidden="1">
+    <row r="227" spans="1:26" ht="80">
       <c r="A227" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T226</v>
@@ -26948,7 +27034,7 @@
       <c r="Y227" s="61"/>
       <c r="Z227" s="61"/>
     </row>
-    <row r="228" spans="1:26" ht="64" hidden="1">
+    <row r="228" spans="1:26" ht="64">
       <c r="A228" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T227</v>
@@ -27007,7 +27093,7 @@
       <c r="Y228" s="61"/>
       <c r="Z228" s="61"/>
     </row>
-    <row r="229" spans="1:26" ht="48" hidden="1">
+    <row r="229" spans="1:26" ht="48">
       <c r="A229" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T228</v>
@@ -27066,7 +27152,7 @@
       <c r="Y229" s="61"/>
       <c r="Z229" s="61"/>
     </row>
-    <row r="230" spans="1:26" ht="80" hidden="1">
+    <row r="230" spans="1:26" ht="80">
       <c r="A230" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T229</v>
@@ -27125,7 +27211,7 @@
       <c r="Y230" s="61"/>
       <c r="Z230" s="61"/>
     </row>
-    <row r="231" spans="1:26" ht="80" hidden="1">
+    <row r="231" spans="1:26" ht="80">
       <c r="A231" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T230</v>
@@ -27184,7 +27270,7 @@
       <c r="Y231" s="61"/>
       <c r="Z231" s="61"/>
     </row>
-    <row r="232" spans="1:26" ht="48" hidden="1">
+    <row r="232" spans="1:26" ht="48">
       <c r="A232" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T231</v>
@@ -27243,7 +27329,7 @@
       <c r="Y232" s="61"/>
       <c r="Z232" s="61"/>
     </row>
-    <row r="233" spans="1:26" ht="96" hidden="1">
+    <row r="233" spans="1:26" ht="96">
       <c r="A233" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T232</v>
@@ -27302,7 +27388,7 @@
       <c r="Y233" s="61"/>
       <c r="Z233" s="61"/>
     </row>
-    <row r="234" spans="1:26" ht="96" hidden="1">
+    <row r="234" spans="1:26" ht="96">
       <c r="A234" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T233</v>
@@ -27361,7 +27447,7 @@
       <c r="Y234" s="61"/>
       <c r="Z234" s="61"/>
     </row>
-    <row r="235" spans="1:26" ht="80" hidden="1">
+    <row r="235" spans="1:26" ht="80">
       <c r="A235" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T234</v>
@@ -27420,7 +27506,7 @@
       <c r="Y235" s="61"/>
       <c r="Z235" s="61"/>
     </row>
-    <row r="236" spans="1:26" ht="80" hidden="1">
+    <row r="236" spans="1:26" ht="80">
       <c r="A236" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T235</v>
@@ -27479,7 +27565,7 @@
       <c r="Y236" s="61"/>
       <c r="Z236" s="61"/>
     </row>
-    <row r="237" spans="1:26" ht="48" hidden="1">
+    <row r="237" spans="1:26" ht="48">
       <c r="A237" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T236</v>
@@ -27538,7 +27624,7 @@
       <c r="Y237" s="61"/>
       <c r="Z237" s="61"/>
     </row>
-    <row r="238" spans="1:26" ht="32" hidden="1">
+    <row r="238" spans="1:26" ht="32">
       <c r="A238" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T237</v>
@@ -27597,7 +27683,7 @@
       <c r="Y238" s="61"/>
       <c r="Z238" s="61"/>
     </row>
-    <row r="239" spans="1:26" ht="80" hidden="1">
+    <row r="239" spans="1:26" ht="80">
       <c r="A239" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T238</v>
@@ -27656,7 +27742,7 @@
       <c r="Y239" s="61"/>
       <c r="Z239" s="61"/>
     </row>
-    <row r="240" spans="1:26" ht="80" hidden="1">
+    <row r="240" spans="1:26" ht="80">
       <c r="A240" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T239</v>
@@ -27715,7 +27801,7 @@
       <c r="Y240" s="61"/>
       <c r="Z240" s="61"/>
     </row>
-    <row r="241" spans="1:26" ht="48" hidden="1">
+    <row r="241" spans="1:26" ht="48">
       <c r="A241" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T240</v>
@@ -27774,7 +27860,7 @@
       <c r="Y241" s="61"/>
       <c r="Z241" s="61"/>
     </row>
-    <row r="242" spans="1:26" ht="32" hidden="1">
+    <row r="242" spans="1:26" ht="32">
       <c r="A242" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T241</v>
@@ -27833,7 +27919,7 @@
       <c r="Y242" s="61"/>
       <c r="Z242" s="61"/>
     </row>
-    <row r="243" spans="1:26" ht="32" hidden="1">
+    <row r="243" spans="1:26" ht="32">
       <c r="A243" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T242</v>
@@ -27892,7 +27978,7 @@
       <c r="Y243" s="61"/>
       <c r="Z243" s="61"/>
     </row>
-    <row r="244" spans="1:26" ht="32" hidden="1">
+    <row r="244" spans="1:26" ht="32">
       <c r="A244" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T243</v>
@@ -27951,7 +28037,7 @@
       <c r="Y244" s="61"/>
       <c r="Z244" s="61"/>
     </row>
-    <row r="245" spans="1:26" ht="80" hidden="1">
+    <row r="245" spans="1:26" ht="80">
       <c r="A245" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T244</v>
@@ -28010,7 +28096,7 @@
       <c r="Y245" s="61"/>
       <c r="Z245" s="61"/>
     </row>
-    <row r="246" spans="1:26" ht="32" hidden="1">
+    <row r="246" spans="1:26" ht="32">
       <c r="A246" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T245</v>
@@ -28069,7 +28155,7 @@
       <c r="Y246" s="61"/>
       <c r="Z246" s="61"/>
     </row>
-    <row r="247" spans="1:26" ht="32" hidden="1">
+    <row r="247" spans="1:26" ht="32">
       <c r="A247" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T246</v>
@@ -28128,7 +28214,7 @@
       <c r="Y247" s="61"/>
       <c r="Z247" s="61"/>
     </row>
-    <row r="248" spans="1:26" ht="80" hidden="1">
+    <row r="248" spans="1:26" ht="80">
       <c r="A248" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T247</v>
@@ -28187,7 +28273,7 @@
       <c r="Y248" s="61"/>
       <c r="Z248" s="61"/>
     </row>
-    <row r="249" spans="1:26" ht="64" hidden="1">
+    <row r="249" spans="1:26" ht="64">
       <c r="A249" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T248</v>
@@ -28246,7 +28332,7 @@
       <c r="Y249" s="61"/>
       <c r="Z249" s="61"/>
     </row>
-    <row r="250" spans="1:26" ht="64" hidden="1">
+    <row r="250" spans="1:26" ht="64">
       <c r="A250" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T249</v>
@@ -28305,7 +28391,7 @@
       <c r="Y250" s="61"/>
       <c r="Z250" s="61"/>
     </row>
-    <row r="251" spans="1:26" ht="96" hidden="1">
+    <row r="251" spans="1:26" ht="96">
       <c r="A251" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T250</v>
@@ -28364,7 +28450,7 @@
       <c r="Y251" s="61"/>
       <c r="Z251" s="61"/>
     </row>
-    <row r="252" spans="1:26" ht="48" hidden="1">
+    <row r="252" spans="1:26" ht="48">
       <c r="A252" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T251</v>
@@ -28423,7 +28509,7 @@
       <c r="Y252" s="61"/>
       <c r="Z252" s="61"/>
     </row>
-    <row r="253" spans="1:26" ht="80" hidden="1">
+    <row r="253" spans="1:26" ht="80">
       <c r="A253" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T252</v>
@@ -28482,7 +28568,7 @@
       <c r="Y253" s="61"/>
       <c r="Z253" s="61"/>
     </row>
-    <row r="254" spans="1:26" ht="16" hidden="1">
+    <row r="254" spans="1:26" ht="16">
       <c r="A254" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T253</v>
@@ -28541,7 +28627,7 @@
       <c r="Y254" s="61"/>
       <c r="Z254" s="61"/>
     </row>
-    <row r="255" spans="1:26" ht="16" hidden="1">
+    <row r="255" spans="1:26" ht="16">
       <c r="A255" s="20" t="str">
         <f t="shared" ref="A255:A269" si="33">CONCATENATE("T",ROW(A255)-1)</f>
         <v>T254</v>
@@ -28626,7 +28712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:26" ht="16" hidden="1">
+    <row r="256" spans="1:26" ht="16">
       <c r="A256" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T255</v>
@@ -28711,7 +28797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:26" ht="16" hidden="1">
+    <row r="257" spans="1:26" ht="16">
       <c r="A257" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T256</v>
@@ -28796,7 +28882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:26" ht="16" hidden="1">
+    <row r="258" spans="1:26" ht="16">
       <c r="A258" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T257</v>
@@ -28881,7 +28967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:26" ht="240" hidden="1">
+    <row r="259" spans="1:26" ht="240">
       <c r="A259" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T258</v>
@@ -28966,7 +29052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:26" ht="16" hidden="1">
+    <row r="260" spans="1:26" ht="16">
       <c r="A260" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T259</v>
@@ -29051,7 +29137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:26" ht="16" hidden="1">
+    <row r="261" spans="1:26" ht="16">
       <c r="A261" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T260</v>
@@ -29136,7 +29222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:26" ht="48" hidden="1">
+    <row r="262" spans="1:26" ht="48">
       <c r="A262" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T261</v>
@@ -29217,7 +29303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:26" ht="32" hidden="1">
+    <row r="263" spans="1:26" ht="32">
       <c r="A263" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T262</v>
@@ -29302,7 +29388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:26" ht="128" hidden="1">
+    <row r="264" spans="1:26" ht="128">
       <c r="A264" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T263</v>
@@ -29387,7 +29473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:26" ht="64" hidden="1">
+    <row r="265" spans="1:26" ht="64">
       <c r="A265" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T264</v>
@@ -29472,7 +29558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:26" ht="48" hidden="1">
+    <row r="266" spans="1:26" ht="48">
       <c r="A266" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T265</v>
@@ -29557,7 +29643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:26" ht="48" hidden="1">
+    <row r="267" spans="1:26" ht="48">
       <c r="A267" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T266</v>
@@ -29638,7 +29724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:26" ht="32" hidden="1">
+    <row r="268" spans="1:26" ht="32">
       <c r="A268" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T267</v>
@@ -29723,7 +29809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:26" ht="32" hidden="1">
+    <row r="269" spans="1:26" ht="32">
       <c r="A269" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T268</v>
@@ -29808,7 +29894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:26" ht="128" hidden="1">
+    <row r="270" spans="1:26" ht="128">
       <c r="A270" s="20" t="str">
         <f t="shared" ref="A270:A313" si="40">CONCATENATE("T",ROW(A270)-1)</f>
         <v>T269</v>
@@ -29877,7 +29963,7 @@
       <c r="Y270" s="61"/>
       <c r="Z270" s="61"/>
     </row>
-    <row r="271" spans="1:26" ht="32" hidden="1">
+    <row r="271" spans="1:26" ht="32">
       <c r="A271" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T270</v>
@@ -29946,7 +30032,7 @@
       <c r="Y271" s="61"/>
       <c r="Z271" s="61"/>
     </row>
-    <row r="272" spans="1:26" ht="96" hidden="1">
+    <row r="272" spans="1:26" ht="96">
       <c r="A272" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T271</v>
@@ -30015,7 +30101,7 @@
       <c r="Y272" s="61"/>
       <c r="Z272" s="61"/>
     </row>
-    <row r="273" spans="1:26" ht="64" hidden="1">
+    <row r="273" spans="1:26" ht="64">
       <c r="A273" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T272</v>
@@ -30084,7 +30170,7 @@
       <c r="Y273" s="61"/>
       <c r="Z273" s="61"/>
     </row>
-    <row r="274" spans="1:26" ht="128" hidden="1">
+    <row r="274" spans="1:26" ht="128">
       <c r="A274" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T273</v>
@@ -30153,7 +30239,7 @@
       <c r="Y274" s="61"/>
       <c r="Z274" s="61"/>
     </row>
-    <row r="275" spans="1:26" ht="96" hidden="1">
+    <row r="275" spans="1:26" ht="96">
       <c r="A275" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T274</v>
@@ -30234,7 +30320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:26" ht="80" hidden="1">
+    <row r="276" spans="1:26" ht="80">
       <c r="A276" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T275</v>
@@ -30315,7 +30401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:26" ht="64" hidden="1">
+    <row r="277" spans="1:26" ht="64">
       <c r="A277" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T276</v>
@@ -30396,7 +30482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:26" ht="96" hidden="1">
+    <row r="278" spans="1:26" ht="96">
       <c r="A278" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T277</v>
@@ -30481,7 +30567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:26" ht="48" hidden="1">
+    <row r="279" spans="1:26" ht="48">
       <c r="A279" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T278</v>
@@ -30562,7 +30648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:26" ht="48" hidden="1">
+    <row r="280" spans="1:26" ht="48">
       <c r="A280" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T279</v>
@@ -30647,7 +30733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:26" ht="48" hidden="1">
+    <row r="281" spans="1:26" ht="48">
       <c r="A281" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T280</v>
@@ -30732,7 +30818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:26" ht="32" hidden="1">
+    <row r="282" spans="1:26" ht="32">
       <c r="A282" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T281</v>
@@ -30817,7 +30903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:26" ht="80" hidden="1">
+    <row r="283" spans="1:26" ht="80">
       <c r="A283" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T282</v>
@@ -30900,7 +30986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:26" ht="160" hidden="1">
+    <row r="284" spans="1:26" ht="160">
       <c r="A284" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T283</v>
@@ -30985,7 +31071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="285" spans="1:26" ht="128" hidden="1">
+    <row r="285" spans="1:26" ht="128">
       <c r="A285" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T284</v>
@@ -31070,7 +31156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="286" spans="1:26" ht="48" hidden="1">
+    <row r="286" spans="1:26" ht="48">
       <c r="A286" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T285</v>
@@ -31155,7 +31241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:26" ht="96" hidden="1">
+    <row r="287" spans="1:26" ht="96">
       <c r="A287" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T286</v>
@@ -31240,7 +31326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:26" ht="96" hidden="1">
+    <row r="288" spans="1:26" ht="96">
       <c r="A288" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T287</v>
@@ -31325,7 +31411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:26" ht="240" hidden="1">
+    <row r="289" spans="1:26" ht="240">
       <c r="A289" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T288</v>
@@ -31410,7 +31496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:26" ht="96" hidden="1">
+    <row r="290" spans="1:26" ht="96">
       <c r="A290" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T289</v>
@@ -31497,7 +31583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:26" ht="176" hidden="1">
+    <row r="291" spans="1:26" ht="176">
       <c r="A291" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T290</v>
@@ -31582,7 +31668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:26" ht="380" hidden="1">
+    <row r="292" spans="1:26" ht="380">
       <c r="A292" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T291</v>
@@ -31667,7 +31753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:26" ht="144" hidden="1">
+    <row r="293" spans="1:26" ht="144">
       <c r="A293" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T292</v>
@@ -31752,7 +31838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:26" ht="112" hidden="1">
+    <row r="294" spans="1:26" ht="112">
       <c r="A294" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T293</v>
@@ -31837,7 +31923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:26" ht="96" hidden="1">
+    <row r="295" spans="1:26" ht="96">
       <c r="A295" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T294</v>
@@ -31922,7 +32008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:26" ht="32" hidden="1">
+    <row r="296" spans="1:26" ht="32">
       <c r="A296" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T295</v>
@@ -32005,7 +32091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:26" ht="32" hidden="1">
+    <row r="297" spans="1:26" ht="32">
       <c r="A297" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T296</v>
@@ -32090,7 +32176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:26" ht="48" hidden="1">
+    <row r="298" spans="1:26" ht="48">
       <c r="A298" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T297</v>
@@ -32175,7 +32261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:26" ht="16" hidden="1">
+    <row r="299" spans="1:26" ht="16">
       <c r="A299" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T298</v>
@@ -32258,7 +32344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:26" ht="16" hidden="1">
+    <row r="300" spans="1:26" ht="16">
       <c r="A300" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T299</v>
@@ -32341,7 +32427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:26" ht="16" hidden="1">
+    <row r="301" spans="1:26" ht="16">
       <c r="A301" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T300</v>
@@ -32424,7 +32510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:26" ht="16" hidden="1">
+    <row r="302" spans="1:26" ht="16">
       <c r="A302" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T301</v>
@@ -32509,7 +32595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="303" spans="1:26" ht="240" hidden="1">
+    <row r="303" spans="1:26" ht="240">
       <c r="A303" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T302</v>
@@ -32594,7 +32680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:26" ht="16" hidden="1">
+    <row r="304" spans="1:26" ht="16">
       <c r="A304" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T303</v>
@@ -32677,7 +32763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:26" ht="16" hidden="1">
+    <row r="305" spans="1:26" ht="16">
       <c r="A305" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T304</v>
@@ -32762,7 +32848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:26" ht="48" hidden="1">
+    <row r="306" spans="1:26" ht="48">
       <c r="A306" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T305</v>
@@ -32843,7 +32929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:26" ht="32" hidden="1">
+    <row r="307" spans="1:26" ht="32">
       <c r="A307" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T306</v>
@@ -32928,7 +33014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:26" ht="128" hidden="1">
+    <row r="308" spans="1:26" ht="128">
       <c r="A308" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T307</v>
@@ -33013,7 +33099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:26" ht="64" hidden="1">
+    <row r="309" spans="1:26" ht="64">
       <c r="A309" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T308</v>
@@ -33098,7 +33184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="310" spans="1:26" ht="48" hidden="1">
+    <row r="310" spans="1:26" ht="48">
       <c r="A310" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T309</v>
@@ -33167,7 +33253,7 @@
       <c r="Y310" s="61"/>
       <c r="Z310" s="61"/>
     </row>
-    <row r="311" spans="1:26" ht="48" hidden="1">
+    <row r="311" spans="1:26" ht="48">
       <c r="A311" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T310</v>
@@ -33232,7 +33318,7 @@
       <c r="Y311" s="61"/>
       <c r="Z311" s="61"/>
     </row>
-    <row r="312" spans="1:26" ht="32" hidden="1">
+    <row r="312" spans="1:26" ht="32">
       <c r="A312" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T311</v>
@@ -33301,7 +33387,7 @@
       <c r="Y312" s="61"/>
       <c r="Z312" s="61"/>
     </row>
-    <row r="313" spans="1:26" ht="16" hidden="1">
+    <row r="313" spans="1:26" ht="16">
       <c r="A313" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T312</v>
@@ -33368,7 +33454,7 @@
       <c r="Y313" s="61"/>
       <c r="Z313" s="61"/>
     </row>
-    <row r="314" spans="1:26" ht="96" hidden="1">
+    <row r="314" spans="1:26" ht="96">
       <c r="A314" s="20" t="str">
         <f t="shared" ref="A314:A320" si="53">CONCATENATE("T",ROW(A314)-1)</f>
         <v>T313</v>
@@ -33427,7 +33513,7 @@
       <c r="Y314" s="61"/>
       <c r="Z314" s="61"/>
     </row>
-    <row r="315" spans="1:26" ht="32" hidden="1">
+    <row r="315" spans="1:26" ht="32">
       <c r="A315" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T314</v>
@@ -33486,7 +33572,7 @@
       <c r="Y315" s="61"/>
       <c r="Z315" s="61"/>
     </row>
-    <row r="316" spans="1:26" ht="80" hidden="1">
+    <row r="316" spans="1:26" ht="80">
       <c r="A316" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T315</v>
@@ -33545,7 +33631,7 @@
       <c r="Y316" s="61"/>
       <c r="Z316" s="61"/>
     </row>
-    <row r="317" spans="1:26" ht="96" hidden="1">
+    <row r="317" spans="1:26" ht="96">
       <c r="A317" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T316</v>
@@ -33604,7 +33690,7 @@
       <c r="Y317" s="61"/>
       <c r="Z317" s="61"/>
     </row>
-    <row r="318" spans="1:26" ht="64" hidden="1">
+    <row r="318" spans="1:26" ht="64">
       <c r="A318" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T317</v>
@@ -33663,7 +33749,7 @@
       <c r="Y318" s="61"/>
       <c r="Z318" s="61"/>
     </row>
-    <row r="319" spans="1:26" ht="112" hidden="1">
+    <row r="319" spans="1:26" ht="112">
       <c r="A319" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T318</v>
@@ -33722,7 +33808,7 @@
       <c r="Y319" s="61"/>
       <c r="Z319" s="61"/>
     </row>
-    <row r="320" spans="1:26" ht="64" hidden="1">
+    <row r="320" spans="1:26" ht="64">
       <c r="A320" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T319</v>
@@ -33781,7 +33867,7 @@
       <c r="Y320" s="61"/>
       <c r="Z320" s="61"/>
     </row>
-    <row r="321" spans="1:26" ht="16" hidden="1">
+    <row r="321" spans="1:26" ht="16">
       <c r="A321" s="20" t="str">
         <f t="shared" ref="A321:A324" si="56">CONCATENATE("T",ROW(A321)-1)</f>
         <v>T320</v>
@@ -33840,7 +33926,7 @@
       <c r="Y321" s="61"/>
       <c r="Z321" s="61"/>
     </row>
-    <row r="322" spans="1:26" ht="80" hidden="1">
+    <row r="322" spans="1:26" ht="80">
       <c r="A322" s="20" t="str">
         <f t="shared" si="56"/>
         <v>T321</v>
@@ -33899,7 +33985,7 @@
       <c r="Y322" s="61"/>
       <c r="Z322" s="61"/>
     </row>
-    <row r="323" spans="1:26" ht="80" hidden="1">
+    <row r="323" spans="1:26" ht="80">
       <c r="A323" s="20" t="str">
         <f t="shared" si="56"/>
         <v>T322</v>
@@ -33949,7 +34035,7 @@
       <c r="Y323" s="61"/>
       <c r="Z323" s="61"/>
     </row>
-    <row r="324" spans="1:26" ht="48" hidden="1">
+    <row r="324" spans="1:26" ht="48">
       <c r="A324" s="20" t="str">
         <f t="shared" si="56"/>
         <v>T323</v>
@@ -33999,7 +34085,7 @@
       <c r="Y324" s="61"/>
       <c r="Z324" s="61"/>
     </row>
-    <row r="325" spans="1:26" ht="48" hidden="1">
+    <row r="325" spans="1:26" ht="48">
       <c r="A325" s="20" t="str">
         <f>CONCATENATE("T",ROW(A325)-1)</f>
         <v>T324</v>
@@ -34049,7 +34135,7 @@
       <c r="Y325" s="61"/>
       <c r="Z325" s="61"/>
     </row>
-    <row r="326" spans="1:26" ht="48" hidden="1">
+    <row r="326" spans="1:26" ht="48">
       <c r="A326" s="20" t="str">
         <f>CONCATENATE("T",ROW(A326)-1)</f>
         <v>T325</v>
@@ -34099,7 +34185,7 @@
       <c r="Y326" s="61"/>
       <c r="Z326" s="61"/>
     </row>
-    <row r="327" spans="1:26" ht="48" hidden="1">
+    <row r="327" spans="1:26" ht="48">
       <c r="A327" s="20" t="str">
         <f t="shared" ref="A327:A332" si="60">CONCATENATE("T",ROW(A327)-1)</f>
         <v>T326</v>
@@ -34149,7 +34235,7 @@
       <c r="Y327" s="61"/>
       <c r="Z327" s="61"/>
     </row>
-    <row r="328" spans="1:26" ht="48" hidden="1">
+    <row r="328" spans="1:26" ht="48">
       <c r="A328" s="20" t="str">
         <f t="shared" si="60"/>
         <v>T327</v>
@@ -34199,7 +34285,7 @@
       <c r="Y328" s="61"/>
       <c r="Z328" s="61"/>
     </row>
-    <row r="329" spans="1:26" ht="48" hidden="1">
+    <row r="329" spans="1:26" ht="48">
       <c r="A329" s="20" t="str">
         <f t="shared" si="60"/>
         <v>T328</v>
@@ -34249,7 +34335,7 @@
       <c r="Y329" s="61"/>
       <c r="Z329" s="61"/>
     </row>
-    <row r="330" spans="1:26" ht="48" hidden="1">
+    <row r="330" spans="1:26" ht="48">
       <c r="A330" s="20" t="str">
         <f t="shared" si="60"/>
         <v>T329</v>
@@ -34299,7 +34385,7 @@
       <c r="Y330" s="61"/>
       <c r="Z330" s="61"/>
     </row>
-    <row r="331" spans="1:26" ht="48" hidden="1">
+    <row r="331" spans="1:26" ht="48">
       <c r="A331" s="20" t="str">
         <f t="shared" si="60"/>
         <v>T330</v>
@@ -34349,7 +34435,7 @@
       <c r="Y331" s="61"/>
       <c r="Z331" s="61"/>
     </row>
-    <row r="332" spans="1:26" ht="48" hidden="1">
+    <row r="332" spans="1:26" ht="48">
       <c r="A332" s="20" t="str">
         <f t="shared" si="60"/>
         <v>T331</v>
@@ -34399,7 +34485,7 @@
       <c r="Y332" s="61"/>
       <c r="Z332" s="61"/>
     </row>
-    <row r="333" spans="1:26" ht="32" hidden="1">
+    <row r="333" spans="1:26" ht="32">
       <c r="A333" s="20" t="str">
         <f>CONCATENATE("T",ROW(A333)-1)</f>
         <v>T332</v>
@@ -34449,7 +34535,7 @@
       <c r="Y333" s="61"/>
       <c r="Z333" s="61"/>
     </row>
-    <row r="334" spans="1:26" ht="48" hidden="1">
+    <row r="334" spans="1:26" ht="48">
       <c r="A334" s="20" t="str">
         <f t="shared" ref="A334:A335" si="61">CONCATENATE("T",ROW(A334)-1)</f>
         <v>T333</v>
@@ -34499,7 +34585,7 @@
       <c r="Y334" s="61"/>
       <c r="Z334" s="61"/>
     </row>
-    <row r="335" spans="1:26" ht="58" hidden="1" customHeight="1">
+    <row r="335" spans="1:26" ht="58" customHeight="1">
       <c r="A335" s="20" t="str">
         <f t="shared" si="61"/>
         <v>T334</v>
@@ -34568,7 +34654,7 @@
       <c r="Y335" s="61"/>
       <c r="Z335" s="61"/>
     </row>
-    <row r="336" spans="1:26" ht="48" hidden="1">
+    <row r="336" spans="1:26" ht="48">
       <c r="A336" s="20" t="str">
         <f>CONCATENATE("T",ROW(A336)-1)</f>
         <v>T335</v>
@@ -34631,7 +34717,7 @@
       <c r="Y336" s="61"/>
       <c r="Z336" s="61"/>
     </row>
-    <row r="337" spans="1:26" ht="96" hidden="1">
+    <row r="337" spans="1:26" ht="96">
       <c r="A337" s="20" t="str">
         <f>CONCATENATE("T",ROW(A337)-1)</f>
         <v>T336</v>
@@ -34694,7 +34780,7 @@
       <c r="Y337" s="61"/>
       <c r="Z337" s="61"/>
     </row>
-    <row r="338" spans="1:26" ht="96" hidden="1">
+    <row r="338" spans="1:26" ht="96">
       <c r="A338" s="20" t="str">
         <f>CONCATENATE("T",ROW(A338)-1)</f>
         <v>T337</v>
@@ -34757,7 +34843,7 @@
       <c r="Y338" s="61"/>
       <c r="Z338" s="61"/>
     </row>
-    <row r="339" spans="1:26" ht="32" hidden="1">
+    <row r="339" spans="1:26" ht="32">
       <c r="A339" s="20" t="str">
         <f t="shared" ref="A339:A341" si="65">CONCATENATE("T",ROW(A339)-1)</f>
         <v>T338</v>
@@ -34823,7 +34909,7 @@
       <c r="Y339" s="61"/>
       <c r="Z339" s="61"/>
     </row>
-    <row r="340" spans="1:26" ht="32" hidden="1">
+    <row r="340" spans="1:26" ht="32">
       <c r="A340" s="20" t="str">
         <f>CONCATENATE("T",ROW(A340)-1)</f>
         <v>T339</v>
@@ -34886,7 +34972,7 @@
       <c r="Y340" s="61"/>
       <c r="Z340" s="61"/>
     </row>
-    <row r="341" spans="1:26" ht="96" hidden="1">
+    <row r="341" spans="1:26" ht="96">
       <c r="A341" s="20" t="str">
         <f t="shared" si="65"/>
         <v>T340</v>
@@ -34955,7 +35041,7 @@
       <c r="Y341" s="61"/>
       <c r="Z341" s="61"/>
     </row>
-    <row r="342" spans="1:26" ht="48" hidden="1">
+    <row r="342" spans="1:26" ht="48">
       <c r="A342" s="20" t="str">
         <f>CONCATENATE("T",ROW(A342)-1)</f>
         <v>T341</v>
@@ -35005,7 +35091,7 @@
       <c r="Y342" s="61"/>
       <c r="Z342" s="61"/>
     </row>
-    <row r="343" spans="1:26" ht="48" hidden="1">
+    <row r="343" spans="1:26" ht="48">
       <c r="A343" s="20" t="str">
         <f t="shared" ref="A343:A355" si="72">CONCATENATE("T",ROW(A343)-1)</f>
         <v>T342</v>
@@ -35055,7 +35141,7 @@
       <c r="Y343" s="61"/>
       <c r="Z343" s="61"/>
     </row>
-    <row r="344" spans="1:26" ht="48" hidden="1">
+    <row r="344" spans="1:26" ht="48">
       <c r="A344" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T343</v>
@@ -35105,7 +35191,7 @@
       <c r="Y344" s="61"/>
       <c r="Z344" s="61"/>
     </row>
-    <row r="345" spans="1:26" ht="48" hidden="1">
+    <row r="345" spans="1:26" ht="48">
       <c r="A345" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T344</v>
@@ -35155,7 +35241,7 @@
       <c r="Y345" s="61"/>
       <c r="Z345" s="61"/>
     </row>
-    <row r="346" spans="1:26" ht="48" hidden="1">
+    <row r="346" spans="1:26" ht="48">
       <c r="A346" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T345</v>
@@ -35205,7 +35291,7 @@
       <c r="Y346" s="61"/>
       <c r="Z346" s="61"/>
     </row>
-    <row r="347" spans="1:26" ht="48" hidden="1">
+    <row r="347" spans="1:26" ht="48">
       <c r="A347" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T346</v>
@@ -35255,7 +35341,7 @@
       <c r="Y347" s="61"/>
       <c r="Z347" s="61"/>
     </row>
-    <row r="348" spans="1:26" ht="64" hidden="1">
+    <row r="348" spans="1:26" ht="64">
       <c r="A348" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T347</v>
@@ -35305,7 +35391,7 @@
       <c r="Y348" s="61"/>
       <c r="Z348" s="61"/>
     </row>
-    <row r="349" spans="1:26" ht="48" hidden="1">
+    <row r="349" spans="1:26" ht="48">
       <c r="A349" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T348</v>
@@ -35355,7 +35441,7 @@
       <c r="Y349" s="61"/>
       <c r="Z349" s="61"/>
     </row>
-    <row r="350" spans="1:26" ht="48" hidden="1">
+    <row r="350" spans="1:26" ht="48">
       <c r="A350" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T349</v>
@@ -35405,7 +35491,7 @@
       <c r="Y350" s="61"/>
       <c r="Z350" s="61"/>
     </row>
-    <row r="351" spans="1:26" ht="48" hidden="1">
+    <row r="351" spans="1:26" ht="48">
       <c r="A351" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T350</v>
@@ -35455,7 +35541,7 @@
       <c r="Y351" s="61"/>
       <c r="Z351" s="61"/>
     </row>
-    <row r="352" spans="1:26" ht="48" hidden="1">
+    <row r="352" spans="1:26" ht="48">
       <c r="A352" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T351</v>
@@ -35505,7 +35591,7 @@
       <c r="Y352" s="61"/>
       <c r="Z352" s="61"/>
     </row>
-    <row r="353" spans="1:26" ht="48" hidden="1">
+    <row r="353" spans="1:26" ht="48">
       <c r="A353" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T352</v>
@@ -35555,7 +35641,7 @@
       <c r="Y353" s="61"/>
       <c r="Z353" s="61"/>
     </row>
-    <row r="354" spans="1:26" ht="48" hidden="1">
+    <row r="354" spans="1:26" ht="48">
       <c r="A354" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T353</v>
@@ -35605,7 +35691,7 @@
       <c r="Y354" s="61"/>
       <c r="Z354" s="61"/>
     </row>
-    <row r="355" spans="1:26" ht="48" hidden="1">
+    <row r="355" spans="1:26" ht="48">
       <c r="A355" s="20" t="str">
         <f t="shared" si="72"/>
         <v>T354</v>
@@ -35655,7 +35741,7 @@
       <c r="Y355" s="61"/>
       <c r="Z355" s="61"/>
     </row>
-    <row r="356" spans="1:26" ht="48" hidden="1">
+    <row r="356" spans="1:26" ht="48">
       <c r="A356" s="20" t="str">
         <f t="shared" ref="A356:A382" si="82">CONCATENATE("T",ROW(A356)-1)</f>
         <v>T355</v>
@@ -35705,7 +35791,7 @@
       <c r="Y356" s="61"/>
       <c r="Z356" s="61"/>
     </row>
-    <row r="357" spans="1:26" ht="48" hidden="1">
+    <row r="357" spans="1:26" ht="48">
       <c r="A357" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T356</v>
@@ -35755,7 +35841,7 @@
       <c r="Y357" s="61"/>
       <c r="Z357" s="61"/>
     </row>
-    <row r="358" spans="1:26" ht="32" hidden="1">
+    <row r="358" spans="1:26" ht="32">
       <c r="A358" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T357</v>
@@ -35805,7 +35891,7 @@
       <c r="Y358" s="61"/>
       <c r="Z358" s="61"/>
     </row>
-    <row r="359" spans="1:26" ht="48" hidden="1">
+    <row r="359" spans="1:26" ht="48">
       <c r="A359" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T358</v>
@@ -35855,7 +35941,7 @@
       <c r="Y359" s="61"/>
       <c r="Z359" s="61"/>
     </row>
-    <row r="360" spans="1:26" ht="32" hidden="1">
+    <row r="360" spans="1:26" ht="32">
       <c r="A360" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T359</v>
@@ -35905,7 +35991,7 @@
       <c r="Y360" s="61"/>
       <c r="Z360" s="61"/>
     </row>
-    <row r="361" spans="1:26" ht="32" hidden="1">
+    <row r="361" spans="1:26" ht="32">
       <c r="A361" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T360</v>
@@ -35955,7 +36041,7 @@
       <c r="Y361" s="61"/>
       <c r="Z361" s="61"/>
     </row>
-    <row r="362" spans="1:26" ht="32" hidden="1">
+    <row r="362" spans="1:26" ht="32">
       <c r="A362" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T361</v>
@@ -36005,7 +36091,7 @@
       <c r="Y362" s="61"/>
       <c r="Z362" s="61"/>
     </row>
-    <row r="363" spans="1:26" ht="32" hidden="1">
+    <row r="363" spans="1:26" ht="32">
       <c r="A363" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T362</v>
@@ -36055,7 +36141,7 @@
       <c r="Y363" s="61"/>
       <c r="Z363" s="61"/>
     </row>
-    <row r="364" spans="1:26" ht="32" hidden="1">
+    <row r="364" spans="1:26" ht="32">
       <c r="A364" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T363</v>
@@ -36105,7 +36191,7 @@
       <c r="Y364" s="61"/>
       <c r="Z364" s="61"/>
     </row>
-    <row r="365" spans="1:26" ht="32" hidden="1">
+    <row r="365" spans="1:26" ht="32">
       <c r="A365" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T364</v>
@@ -36155,7 +36241,7 @@
       <c r="Y365" s="61"/>
       <c r="Z365" s="61"/>
     </row>
-    <row r="366" spans="1:26" ht="32" hidden="1">
+    <row r="366" spans="1:26" ht="32">
       <c r="A366" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T365</v>
@@ -36205,7 +36291,7 @@
       <c r="Y366" s="61"/>
       <c r="Z366" s="61"/>
     </row>
-    <row r="367" spans="1:26" ht="32" hidden="1">
+    <row r="367" spans="1:26" ht="32">
       <c r="A367" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T366</v>
@@ -36255,7 +36341,7 @@
       <c r="Y367" s="61"/>
       <c r="Z367" s="61"/>
     </row>
-    <row r="368" spans="1:26" ht="32" hidden="1">
+    <row r="368" spans="1:26" ht="32">
       <c r="A368" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T367</v>
@@ -36305,7 +36391,7 @@
       <c r="Y368" s="61"/>
       <c r="Z368" s="61"/>
     </row>
-    <row r="369" spans="1:26" ht="48" hidden="1">
+    <row r="369" spans="1:26" ht="48">
       <c r="A369" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T368</v>
@@ -36355,7 +36441,7 @@
       <c r="Y369" s="61"/>
       <c r="Z369" s="61"/>
     </row>
-    <row r="370" spans="1:26" ht="48" hidden="1">
+    <row r="370" spans="1:26" ht="48">
       <c r="A370" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T369</v>
@@ -36407,7 +36493,7 @@
       <c r="Y370" s="61"/>
       <c r="Z370" s="61"/>
     </row>
-    <row r="371" spans="1:26" ht="48" hidden="1">
+    <row r="371" spans="1:26" ht="48">
       <c r="A371" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T370</v>
@@ -36457,7 +36543,7 @@
       <c r="Y371" s="61"/>
       <c r="Z371" s="61"/>
     </row>
-    <row r="372" spans="1:26" ht="48" hidden="1">
+    <row r="372" spans="1:26" ht="48">
       <c r="A372" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T371</v>
@@ -36507,7 +36593,7 @@
       <c r="Y372" s="61"/>
       <c r="Z372" s="61"/>
     </row>
-    <row r="373" spans="1:26" ht="48" hidden="1">
+    <row r="373" spans="1:26" ht="48">
       <c r="A373" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T372</v>
@@ -36557,7 +36643,7 @@
       <c r="Y373" s="61"/>
       <c r="Z373" s="61"/>
     </row>
-    <row r="374" spans="1:26" ht="48" hidden="1">
+    <row r="374" spans="1:26" ht="48">
       <c r="A374" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T373</v>
@@ -36607,7 +36693,7 @@
       <c r="Y374" s="61"/>
       <c r="Z374" s="61"/>
     </row>
-    <row r="375" spans="1:26" ht="80" hidden="1">
+    <row r="375" spans="1:26" ht="80">
       <c r="A375" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T374</v>
@@ -36671,7 +36757,7 @@
       <c r="Y375" s="61"/>
       <c r="Z375" s="61"/>
     </row>
-    <row r="376" spans="1:26" ht="32" hidden="1">
+    <row r="376" spans="1:26" ht="32">
       <c r="A376" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T375</v>
@@ -36725,7 +36811,7 @@
       <c r="Y376" s="61"/>
       <c r="Z376" s="61"/>
     </row>
-    <row r="377" spans="1:26" ht="32" hidden="1">
+    <row r="377" spans="1:26" ht="32">
       <c r="A377" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T376</v>
@@ -36779,7 +36865,7 @@
       <c r="Y377" s="61"/>
       <c r="Z377" s="61"/>
     </row>
-    <row r="378" spans="1:26" ht="32" hidden="1">
+    <row r="378" spans="1:26" ht="32">
       <c r="A378" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T377</v>
@@ -36833,7 +36919,7 @@
       <c r="Y378" s="61"/>
       <c r="Z378" s="61"/>
     </row>
-    <row r="379" spans="1:26" ht="32" hidden="1">
+    <row r="379" spans="1:26" ht="32">
       <c r="A379" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T378</v>
@@ -36885,7 +36971,7 @@
       <c r="Y379" s="61"/>
       <c r="Z379" s="61"/>
     </row>
-    <row r="380" spans="1:26" ht="32" hidden="1">
+    <row r="380" spans="1:26" ht="32">
       <c r="A380" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T379</v>
@@ -36937,7 +37023,7 @@
       <c r="Y380" s="61"/>
       <c r="Z380" s="61"/>
     </row>
-    <row r="381" spans="1:26" ht="32" hidden="1">
+    <row r="381" spans="1:26" ht="32">
       <c r="A381" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T380</v>
@@ -36989,7 +37075,7 @@
       <c r="Y381" s="61"/>
       <c r="Z381" s="61"/>
     </row>
-    <row r="382" spans="1:26" ht="32" hidden="1">
+    <row r="382" spans="1:26" ht="32">
       <c r="A382" s="20" t="str">
         <f t="shared" si="82"/>
         <v>T381</v>
@@ -37041,7 +37127,7 @@
       <c r="Y382" s="61"/>
       <c r="Z382" s="61"/>
     </row>
-    <row r="383" spans="1:26" ht="32" hidden="1">
+    <row r="383" spans="1:26" ht="32">
       <c r="A383" s="20" t="str">
         <f>CONCATENATE("T",ROW(A383)-1)</f>
         <v>T382</v>
@@ -37105,7 +37191,7 @@
       <c r="Y383" s="61"/>
       <c r="Z383" s="61"/>
     </row>
-    <row r="384" spans="1:26" ht="96" hidden="1">
+    <row r="384" spans="1:26" ht="96">
       <c r="A384" s="20" t="str">
         <f>CONCATENATE("T",ROW(A384)-1)</f>
         <v>T383</v>
@@ -37174,7 +37260,7 @@
       <c r="Y384" s="61"/>
       <c r="Z384" s="61"/>
     </row>
-    <row r="385" spans="1:26" ht="48" hidden="1">
+    <row r="385" spans="1:26" ht="48">
       <c r="A385" s="20" t="str">
         <f t="shared" ref="A385:A388" si="93">CONCATENATE("T",ROW(A385)-1)</f>
         <v>T384</v>
@@ -37239,7 +37325,7 @@
       <c r="Y385" s="61"/>
       <c r="Z385" s="61"/>
     </row>
-    <row r="386" spans="1:26" ht="48" hidden="1">
+    <row r="386" spans="1:26" ht="48">
       <c r="A386" s="20" t="str">
         <f t="shared" si="93"/>
         <v>T385</v>
@@ -37308,7 +37394,7 @@
       <c r="Y386" s="61"/>
       <c r="Z386" s="61"/>
     </row>
-    <row r="387" spans="1:26" ht="48" hidden="1">
+    <row r="387" spans="1:26" ht="48">
       <c r="A387" s="20" t="str">
         <f t="shared" si="93"/>
         <v>T386</v>
@@ -37377,7 +37463,7 @@
       <c r="Y387" s="61"/>
       <c r="Z387" s="61"/>
     </row>
-    <row r="388" spans="1:26" ht="32" hidden="1">
+    <row r="388" spans="1:26" ht="32">
       <c r="A388" s="20" t="str">
         <f t="shared" si="93"/>
         <v>T387</v>
@@ -37446,7 +37532,7 @@
       <c r="Y388" s="61"/>
       <c r="Z388" s="61"/>
     </row>
-    <row r="389" spans="1:26" ht="160" hidden="1">
+    <row r="389" spans="1:26" ht="160">
       <c r="A389" s="20" t="str">
         <f t="shared" ref="A389:A393" si="94">CONCATENATE("T",ROW(A389)-1)</f>
         <v>T388</v>
@@ -37515,7 +37601,7 @@
       <c r="Y389" s="61"/>
       <c r="Z389" s="61"/>
     </row>
-    <row r="390" spans="1:26" ht="128" hidden="1">
+    <row r="390" spans="1:26" ht="128">
       <c r="A390" s="20" t="str">
         <f t="shared" si="94"/>
         <v>T389</v>
@@ -37584,7 +37670,7 @@
       <c r="Y390" s="61"/>
       <c r="Z390" s="61"/>
     </row>
-    <row r="391" spans="1:26" ht="96" hidden="1">
+    <row r="391" spans="1:26" ht="96">
       <c r="A391" s="20" t="str">
         <f t="shared" si="94"/>
         <v>T390</v>
@@ -37653,7 +37739,7 @@
       <c r="Y391" s="61"/>
       <c r="Z391" s="61"/>
     </row>
-    <row r="392" spans="1:26" ht="96" hidden="1">
+    <row r="392" spans="1:26" ht="96">
       <c r="A392" s="20" t="str">
         <f t="shared" si="94"/>
         <v>T391</v>
@@ -37722,7 +37808,7 @@
       <c r="Y392" s="61"/>
       <c r="Z392" s="61"/>
     </row>
-    <row r="393" spans="1:26" ht="240" hidden="1">
+    <row r="393" spans="1:26" ht="240">
       <c r="A393" s="20" t="str">
         <f t="shared" si="94"/>
         <v>T392</v>
@@ -37790,6 +37876,1185 @@
       <c r="X393" s="61"/>
       <c r="Y393" s="61"/>
       <c r="Z393" s="61"/>
+    </row>
+    <row r="394" spans="1:26" ht="96">
+      <c r="A394" s="75" t="str">
+        <f>CONCATENATE("T",ROW(A394)-1)</f>
+        <v>T393</v>
+      </c>
+      <c r="B394" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C394" s="56" t="s">
+        <v>641</v>
+      </c>
+      <c r="D394" s="56" t="s">
+        <v>642</v>
+      </c>
+      <c r="E394" s="56" t="s">
+        <v>391</v>
+      </c>
+      <c r="F394" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G394" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H394" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I394" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J394" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K394" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="L394" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="M394" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="N394" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="O394" s="70" t="s">
+        <v>643</v>
+      </c>
+      <c r="P394" s="70" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q394" s="70" t="s">
+        <v>645</v>
+      </c>
+      <c r="R394" s="70"/>
+      <c r="S394" s="76">
+        <v>5</v>
+      </c>
+      <c r="T394" s="76">
+        <v>6</v>
+      </c>
+      <c r="U394" s="76">
+        <v>5</v>
+      </c>
+      <c r="V394" s="76">
+        <v>5</v>
+      </c>
+      <c r="W394" s="76">
+        <v>7</v>
+      </c>
+      <c r="X394" s="76">
+        <v>7</v>
+      </c>
+      <c r="Y394" s="76">
+        <v>6</v>
+      </c>
+      <c r="Z394" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="395" spans="1:26" ht="80">
+      <c r="A395" s="75" t="str">
+        <f t="shared" ref="A395:A408" si="95">CONCATENATE("T",ROW(A395)-1)</f>
+        <v>T394</v>
+      </c>
+      <c r="B395" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C395" s="71" t="s">
+        <v>646</v>
+      </c>
+      <c r="D395" s="71" t="s">
+        <v>647</v>
+      </c>
+      <c r="E395" s="71" t="s">
+        <v>648</v>
+      </c>
+      <c r="F395" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="G395" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H395" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I395" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J395" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K395" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="L395" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="M395" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="N395" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O395" s="72" t="s">
+        <v>649</v>
+      </c>
+      <c r="P395" s="72" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q395" s="72" t="s">
+        <v>651</v>
+      </c>
+      <c r="R395" s="73"/>
+      <c r="S395" s="77">
+        <v>6</v>
+      </c>
+      <c r="T395" s="77">
+        <v>5</v>
+      </c>
+      <c r="U395" s="77">
+        <v>5</v>
+      </c>
+      <c r="V395" s="77">
+        <v>4</v>
+      </c>
+      <c r="W395" s="77">
+        <v>8</v>
+      </c>
+      <c r="X395" s="77">
+        <v>6</v>
+      </c>
+      <c r="Y395" s="77">
+        <v>5</v>
+      </c>
+      <c r="Z395" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="396" spans="1:26" ht="64">
+      <c r="A396" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T395</v>
+      </c>
+      <c r="B396" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C396" s="56" t="s">
+        <v>652</v>
+      </c>
+      <c r="D396" s="56" t="s">
+        <v>653</v>
+      </c>
+      <c r="E396" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="F396" s="56" t="s">
+        <v>403</v>
+      </c>
+      <c r="G396" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H396" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I396" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J396" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K396" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="L396" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="M396" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="N396" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="O396" s="74" t="s">
+        <v>654</v>
+      </c>
+      <c r="P396" s="74" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q396" s="74" t="s">
+        <v>656</v>
+      </c>
+      <c r="R396" s="70"/>
+      <c r="S396" s="76">
+        <v>5</v>
+      </c>
+      <c r="T396" s="76">
+        <v>6</v>
+      </c>
+      <c r="U396" s="76">
+        <v>5</v>
+      </c>
+      <c r="V396" s="76">
+        <v>6</v>
+      </c>
+      <c r="W396" s="76">
+        <v>9</v>
+      </c>
+      <c r="X396" s="76">
+        <v>7</v>
+      </c>
+      <c r="Y396" s="76">
+        <v>7</v>
+      </c>
+      <c r="Z396" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="397" spans="1:26" ht="96">
+      <c r="A397" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T396</v>
+      </c>
+      <c r="B397" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C397" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="D397" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="E397" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="F397" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G397" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I397" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J397" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K397" s="71" t="s">
+        <v>1642</v>
+      </c>
+      <c r="L397" s="71" t="s">
+        <v>1642</v>
+      </c>
+      <c r="M397" s="71" t="s">
+        <v>1643</v>
+      </c>
+      <c r="N397" s="71" t="s">
+        <v>657</v>
+      </c>
+      <c r="O397" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="P397" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="Q397" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="R397" s="73"/>
+      <c r="S397" s="77">
+        <v>8</v>
+      </c>
+      <c r="T397" s="77">
+        <v>7</v>
+      </c>
+      <c r="U397" s="77">
+        <v>6</v>
+      </c>
+      <c r="V397" s="77">
+        <v>5</v>
+      </c>
+      <c r="W397" s="77">
+        <v>9</v>
+      </c>
+      <c r="X397" s="77">
+        <v>8</v>
+      </c>
+      <c r="Y397" s="77">
+        <v>6</v>
+      </c>
+      <c r="Z397" s="79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="398" spans="1:26" ht="48">
+      <c r="A398" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T397</v>
+      </c>
+      <c r="B398" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C398" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D398" s="56" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E398" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F398" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G398" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H398" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I398" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J398" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K398" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="L398" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="M398" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="N398" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="O398" s="57"/>
+      <c r="P398" s="57"/>
+      <c r="Q398" s="57"/>
+      <c r="R398" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="S398" s="76">
+        <v>6</v>
+      </c>
+      <c r="T398" s="76">
+        <v>6</v>
+      </c>
+      <c r="U398" s="76">
+        <v>5</v>
+      </c>
+      <c r="V398" s="76">
+        <v>6</v>
+      </c>
+      <c r="W398" s="76">
+        <v>3</v>
+      </c>
+      <c r="X398" s="76">
+        <v>4</v>
+      </c>
+      <c r="Y398" s="76">
+        <v>9</v>
+      </c>
+      <c r="Z398" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="399" spans="1:26" ht="48">
+      <c r="A399" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T398</v>
+      </c>
+      <c r="B399" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C399" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="D399" s="71" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E399" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F399" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G399" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H399" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I399" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J399" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K399" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="L399" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="M399" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="N399" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="O399" s="73" t="s">
+        <v>237</v>
+      </c>
+      <c r="P399" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q399" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="R399" s="73"/>
+      <c r="S399" s="77">
+        <v>6</v>
+      </c>
+      <c r="T399" s="77">
+        <v>6</v>
+      </c>
+      <c r="U399" s="77">
+        <v>5</v>
+      </c>
+      <c r="V399" s="77">
+        <v>5</v>
+      </c>
+      <c r="W399" s="77">
+        <v>8</v>
+      </c>
+      <c r="X399" s="77">
+        <v>7</v>
+      </c>
+      <c r="Y399" s="77">
+        <v>5</v>
+      </c>
+      <c r="Z399" s="79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="400" spans="1:26" ht="48">
+      <c r="A400" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T399</v>
+      </c>
+      <c r="B400" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C400" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="D400" s="56" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E400" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F400" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G400" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H400" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I400" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J400" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K400" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="L400" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="M400" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="N400" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="O400" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="P400" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q400" s="70" t="s">
+        <v>244</v>
+      </c>
+      <c r="R400" s="70"/>
+      <c r="S400" s="76">
+        <v>6</v>
+      </c>
+      <c r="T400" s="76">
+        <v>6</v>
+      </c>
+      <c r="U400" s="76">
+        <v>5</v>
+      </c>
+      <c r="V400" s="76">
+        <v>5</v>
+      </c>
+      <c r="W400" s="76">
+        <v>8</v>
+      </c>
+      <c r="X400" s="76">
+        <v>7</v>
+      </c>
+      <c r="Y400" s="76">
+        <v>6</v>
+      </c>
+      <c r="Z400" s="78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="401" spans="1:26" ht="32">
+      <c r="A401" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T400</v>
+      </c>
+      <c r="B401" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C401" s="71" t="s">
+        <v>661</v>
+      </c>
+      <c r="D401" s="71" t="s">
+        <v>246</v>
+      </c>
+      <c r="E401" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F401" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G401" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H401" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I401" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J401" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K401" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="L401" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="M401" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="N401" s="71" t="s">
+        <v>247</v>
+      </c>
+      <c r="O401" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="P401" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q401" s="73" t="s">
+        <v>250</v>
+      </c>
+      <c r="R401" s="73"/>
+      <c r="S401" s="77">
+        <v>5</v>
+      </c>
+      <c r="T401" s="77">
+        <v>6</v>
+      </c>
+      <c r="U401" s="77">
+        <v>5</v>
+      </c>
+      <c r="V401" s="77">
+        <v>6</v>
+      </c>
+      <c r="W401" s="77">
+        <v>7</v>
+      </c>
+      <c r="X401" s="77">
+        <v>9</v>
+      </c>
+      <c r="Y401" s="77">
+        <v>5</v>
+      </c>
+      <c r="Z401" s="79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="402" spans="1:26" ht="80">
+      <c r="A402" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T401</v>
+      </c>
+      <c r="B402" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C402" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D402" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="E402" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F402" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G402" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="H402" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="I402" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J402" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="K402" s="56" t="s">
+        <v>1642</v>
+      </c>
+      <c r="L402" s="56" t="s">
+        <v>1642</v>
+      </c>
+      <c r="M402" s="56" t="s">
+        <v>1643</v>
+      </c>
+      <c r="N402" s="56" t="s">
+        <v>662</v>
+      </c>
+      <c r="O402" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="P402" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q402" s="57"/>
+      <c r="R402" s="70"/>
+      <c r="S402" s="76">
+        <v>5</v>
+      </c>
+      <c r="T402" s="76">
+        <v>6</v>
+      </c>
+      <c r="U402" s="76">
+        <v>5</v>
+      </c>
+      <c r="V402" s="76">
+        <v>6</v>
+      </c>
+      <c r="W402" s="76">
+        <v>3</v>
+      </c>
+      <c r="X402" s="76">
+        <v>4</v>
+      </c>
+      <c r="Y402" s="76">
+        <v>9</v>
+      </c>
+      <c r="Z402" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="403" spans="1:26" ht="160">
+      <c r="A403" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T402</v>
+      </c>
+      <c r="B403" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C403" s="71" t="s">
+        <v>255</v>
+      </c>
+      <c r="D403" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="E403" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F403" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G403" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H403" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I403" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J403" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K403" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="L403" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="M403" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="N403" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="O403" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="P403" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q403" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="R403" s="73"/>
+      <c r="S403" s="77">
+        <v>6</v>
+      </c>
+      <c r="T403" s="77">
+        <v>7</v>
+      </c>
+      <c r="U403" s="77">
+        <v>5</v>
+      </c>
+      <c r="V403" s="77">
+        <v>5</v>
+      </c>
+      <c r="W403" s="77">
+        <v>8</v>
+      </c>
+      <c r="X403" s="77">
+        <v>8</v>
+      </c>
+      <c r="Y403" s="77">
+        <v>6</v>
+      </c>
+      <c r="Z403" s="79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="404" spans="1:26" ht="128">
+      <c r="A404" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T403</v>
+      </c>
+      <c r="B404" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C404" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="D404" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="E404" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F404" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G404" s="56" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H404" s="56" t="s">
+        <v>1642</v>
+      </c>
+      <c r="I404" s="56" t="s">
+        <v>1643</v>
+      </c>
+      <c r="J404" s="56" t="s">
+        <v>663</v>
+      </c>
+      <c r="K404" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="L404" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="M404" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="N404" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="O404" s="74" t="s">
+        <v>664</v>
+      </c>
+      <c r="P404" s="74" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q404" s="74" t="s">
+        <v>666</v>
+      </c>
+      <c r="R404" s="70"/>
+      <c r="S404" s="76">
+        <v>7</v>
+      </c>
+      <c r="T404" s="76">
+        <v>6</v>
+      </c>
+      <c r="U404" s="76">
+        <v>8</v>
+      </c>
+      <c r="V404" s="76">
+        <v>6</v>
+      </c>
+      <c r="W404" s="76">
+        <v>9</v>
+      </c>
+      <c r="X404" s="76">
+        <v>9</v>
+      </c>
+      <c r="Y404" s="76">
+        <v>7</v>
+      </c>
+      <c r="Z404" s="78">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="405" spans="1:26" ht="48">
+      <c r="A405" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T404</v>
+      </c>
+      <c r="B405" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C405" s="71" t="s">
+        <v>293</v>
+      </c>
+      <c r="D405" s="71" t="s">
+        <v>667</v>
+      </c>
+      <c r="E405" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F405" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G405" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="H405" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="I405" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J405" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="K405" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="L405" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="M405" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="N405" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="O405" s="73" t="s">
+        <v>363</v>
+      </c>
+      <c r="P405" s="73" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q405" s="73" t="s">
+        <v>669</v>
+      </c>
+      <c r="R405" s="73"/>
+      <c r="S405" s="77">
+        <v>5</v>
+      </c>
+      <c r="T405" s="77">
+        <v>7</v>
+      </c>
+      <c r="U405" s="77">
+        <v>6</v>
+      </c>
+      <c r="V405" s="77">
+        <v>6</v>
+      </c>
+      <c r="W405" s="77">
+        <v>2</v>
+      </c>
+      <c r="X405" s="77">
+        <v>4</v>
+      </c>
+      <c r="Y405" s="77">
+        <v>9</v>
+      </c>
+      <c r="Z405" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="406" spans="1:26" ht="96">
+      <c r="A406" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T405</v>
+      </c>
+      <c r="B406" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C406" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="D406" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="E406" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F406" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="G406" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H406" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I406" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="J406" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K406" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="L406" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="M406" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="N406" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="O406" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="P406" s="74" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q406" s="74" t="s">
+        <v>671</v>
+      </c>
+      <c r="R406" s="70"/>
+      <c r="S406" s="76">
+        <v>5</v>
+      </c>
+      <c r="T406" s="76">
+        <v>7</v>
+      </c>
+      <c r="U406" s="76">
+        <v>6</v>
+      </c>
+      <c r="V406" s="76">
+        <v>6</v>
+      </c>
+      <c r="W406" s="76">
+        <v>6</v>
+      </c>
+      <c r="X406" s="76">
+        <v>9</v>
+      </c>
+      <c r="Y406" s="76">
+        <v>6</v>
+      </c>
+      <c r="Z406" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="407" spans="1:26" ht="96">
+      <c r="A407" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T406</v>
+      </c>
+      <c r="B407" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C407" s="71" t="s">
+        <v>274</v>
+      </c>
+      <c r="D407" s="71" t="s">
+        <v>275</v>
+      </c>
+      <c r="E407" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="F407" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="G407" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="H407" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I407" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J407" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K407" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="L407" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="M407" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="N407" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="O407" s="73" t="s">
+        <v>276</v>
+      </c>
+      <c r="P407" s="73" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q407" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="R407" s="73"/>
+      <c r="S407" s="77">
+        <v>6</v>
+      </c>
+      <c r="T407" s="77">
+        <v>8</v>
+      </c>
+      <c r="U407" s="77">
+        <v>6</v>
+      </c>
+      <c r="V407" s="77">
+        <v>6</v>
+      </c>
+      <c r="W407" s="77">
+        <v>7</v>
+      </c>
+      <c r="X407" s="77">
+        <v>9</v>
+      </c>
+      <c r="Y407" s="77">
+        <v>6</v>
+      </c>
+      <c r="Z407" s="79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="408" spans="1:26" ht="240">
+      <c r="A408" s="75" t="str">
+        <f t="shared" si="95"/>
+        <v>T407</v>
+      </c>
+      <c r="B408" s="56" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C408" s="80" t="s">
+        <v>279</v>
+      </c>
+      <c r="D408" s="80" t="s">
+        <v>280</v>
+      </c>
+      <c r="E408" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="F408" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="G408" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="H408" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="I408" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="J408" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="K408" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="L408" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="M408" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="N408" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="O408" s="81" t="s">
+        <v>281</v>
+      </c>
+      <c r="P408" s="81" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q408" s="81" t="s">
+        <v>283</v>
+      </c>
+      <c r="R408" s="81"/>
+      <c r="S408" s="82">
+        <v>6</v>
+      </c>
+      <c r="T408" s="82">
+        <v>5</v>
+      </c>
+      <c r="U408" s="82">
+        <v>5</v>
+      </c>
+      <c r="V408" s="82">
+        <v>5</v>
+      </c>
+      <c r="W408" s="82">
+        <v>6</v>
+      </c>
+      <c r="X408" s="82">
+        <v>4</v>
+      </c>
+      <c r="Y408" s="82">
+        <v>4</v>
+      </c>
+      <c r="Z408" s="83">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -45321,8 +46586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>

</xml_diff>